<commit_message>
check README.txt for updated chages
</commit_message>
<xml_diff>
--- a/panda_test.xlsx
+++ b/panda_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="174">
   <si>
     <t>M</t>
   </si>
@@ -28,43 +28,28 @@
     <t>M2</t>
   </si>
   <si>
-    <t>Evolutionary Rxn</t>
-  </si>
-  <si>
-    <t>GLY-DC_Lt_m</t>
-  </si>
-  <si>
-    <t>GLY-DC_Dk_m</t>
-  </si>
-  <si>
-    <t>PEPCase_Lt_c</t>
-  </si>
-  <si>
-    <t>PEPCase_Dk_c</t>
-  </si>
-  <si>
-    <t>CA_Lt_c</t>
-  </si>
-  <si>
-    <t>CA_Dk_c</t>
-  </si>
-  <si>
-    <t>Rubisco-Carbox_Lt_p</t>
-  </si>
-  <si>
-    <t>Rubisco-Carbox_Dk_p</t>
-  </si>
-  <si>
-    <t>Rubisco-Oxy_Lt_p</t>
-  </si>
-  <si>
-    <t>Rubisco-Oxy_Dk_p</t>
-  </si>
-  <si>
-    <t>NADP-ME_Lt_c</t>
-  </si>
-  <si>
-    <t>NADP-ME_Dk_c</t>
+    <t>Malate_Lt_M1M2</t>
+  </si>
+  <si>
+    <t>Malate_Dk_M1M2</t>
+  </si>
+  <si>
+    <t>Pyruvate_Lt_M1M2</t>
+  </si>
+  <si>
+    <t>Pyruvate_Dk_M1M2</t>
+  </si>
+  <si>
+    <t>Sucrose_Light_M1M2</t>
+  </si>
+  <si>
+    <t>Sucrose_Dark_M1M2</t>
+  </si>
+  <si>
+    <t>GLY_Light_M1M2</t>
+  </si>
+  <si>
+    <t>GLY_Dark_M1M2</t>
   </si>
   <si>
     <t>GLYCOLYSIS</t>
@@ -452,30 +437,6 @@
   </si>
   <si>
     <t>O2_Dark_tx</t>
-  </si>
-  <si>
-    <t>Malate_Lt_M1M2</t>
-  </si>
-  <si>
-    <t>Malate_Dk_M1M2</t>
-  </si>
-  <si>
-    <t>Pyruvate_Lt_M1M2</t>
-  </si>
-  <si>
-    <t>Pyruvate_Dk_M1M2</t>
-  </si>
-  <si>
-    <t>Sucrose_Light_M1M2</t>
-  </si>
-  <si>
-    <t>Sucrose_Dark_M1M2</t>
-  </si>
-  <si>
-    <t>GLY_Light_M1M2</t>
-  </si>
-  <si>
-    <t>GLY_Dark_M1M2</t>
   </si>
   <si>
     <t>MET_Light_M1M2</t>
@@ -932,7 +893,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F228"/>
+  <dimension ref="B1:F223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -956,120 +917,72 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>186</v>
+      <c r="E2">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>2.46541525830547</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>3.66471116431321</v>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>0.00599475931482119</v>
-      </c>
-      <c r="D4">
-        <v>0.0131585445355179</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="E4">
+        <v>-43.8942882190986</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>0.236676211909824</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
+      <c r="E5">
+        <v>1.11978422241723</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
+      <c r="E6">
+        <v>0.587747532929956</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
-        <v>0.236676211909824</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
+      <c r="E7">
+        <v>0.28855520120963</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
+      <c r="E8">
+        <v>-1.99837724167508</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
-        <v>14.8163148790579</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>30</v>
+      <c r="E9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
+      <c r="C10" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="2:6">
@@ -1077,13 +990,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>4.93877162635264</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -1125,15 +1038,21 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0.145317099796486</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
-        <v>186</v>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>-0.042404065483858</v>
       </c>
     </row>
     <row r="16" spans="2:6">
@@ -1147,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>1.47165233828602</v>
+        <v>-0.042404065483858</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -1155,13 +1074,13 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>-1.2018036174373</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>-1.76919890724782</v>
       </c>
       <c r="F17">
-        <v>0.654712533196115</v>
+        <v>-0.473168200022645</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -1169,13 +1088,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>-1.2018036174373</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>-1.76919890724782</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>-0.473168200022645</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -1203,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>-4.72531330758772</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:6">
@@ -1217,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>-4.72531330758772</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:6">
@@ -1225,13 +1144,13 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>-1.20180361756454</v>
+        <v>0.0268756059410347</v>
       </c>
       <c r="D22">
-        <v>-4.67768415098149</v>
+        <v>0.0264577059376176</v>
       </c>
       <c r="F22">
-        <v>8.46211513547727</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:6">
@@ -1239,13 +1158,13 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>-1.20180361756454</v>
+        <v>-0.685115350149317</v>
       </c>
       <c r="D23">
-        <v>-4.67768415098149</v>
+        <v>-0.876302734139586</v>
       </c>
       <c r="F23">
-        <v>8.46211513547727</v>
+        <v>-0.124044341583801</v>
       </c>
     </row>
     <row r="24" spans="2:6">
@@ -1253,13 +1172,13 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>0.17127883753733</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>0.300421621460615</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>-0.0654259315329966</v>
       </c>
     </row>
     <row r="25" spans="2:6">
@@ -1267,13 +1186,13 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>-7.79357979984874</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>-1.67109711155474</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>-13.6701065583721</v>
       </c>
     </row>
     <row r="26" spans="2:6">
@@ -1281,10 +1200,10 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>0.0268756059410347</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>0.0264577059376176</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1295,13 +1214,13 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>0.0268756059235726</v>
+        <v>0.685115350149317</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>0.876302734139586</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>0.124044341583801</v>
       </c>
     </row>
     <row r="28" spans="2:6">
@@ -1309,13 +1228,13 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>-0.685115350265279</v>
+        <v>-0.198154443478364</v>
       </c>
       <c r="D28">
-        <v>-3.75891089584869</v>
+        <v>-0.300421621460615</v>
       </c>
       <c r="F28">
-        <v>-4.72531330758772</v>
+        <v>0.0654259315329966</v>
       </c>
     </row>
     <row r="29" spans="2:6">
@@ -1323,13 +1242,13 @@
         <v>31</v>
       </c>
       <c r="C29">
-        <v>0.171278837566319</v>
+        <v>14.3772591644857</v>
       </c>
       <c r="D29">
-        <v>-0.186278669032052</v>
+        <v>1.67109711155474</v>
       </c>
       <c r="F29">
-        <v>0.486058975727367</v>
+        <v>26.8564969876096</v>
       </c>
     </row>
     <row r="30" spans="2:6">
@@ -1337,13 +1256,13 @@
         <v>32</v>
       </c>
       <c r="C30">
-        <v>-7.79357980084795</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>-4.20715971820001</v>
+        <v>-0.0264577059376176</v>
       </c>
       <c r="F30">
-        <v>-4.59344042007828</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:6">
@@ -1351,7 +1270,7 @@
         <v>33</v>
       </c>
       <c r="C31">
-        <v>0.0268756059235726</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1365,13 +1284,13 @@
         <v>34</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>0.70140490779583</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1.05442425662798</v>
       </c>
       <c r="F32">
-        <v>15.0892989085049</v>
+        <v>0.0654259315329985</v>
       </c>
     </row>
     <row r="33" spans="2:6">
@@ -1379,13 +1298,13 @@
         <v>35</v>
       </c>
       <c r="C33">
-        <v>-0.171278837566319</v>
+        <v>-0.00529407316024472</v>
       </c>
       <c r="D33">
-        <v>0.186278669032051</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>-0.486058975727367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:6">
@@ -1393,13 +1312,13 @@
         <v>36</v>
       </c>
       <c r="C34">
-        <v>15.0623745166208</v>
+        <v>0.0134378029705174</v>
       </c>
       <c r="D34">
-        <v>7.96607061404871</v>
+        <v>0.0165757920139583</v>
       </c>
       <c r="F34">
-        <v>7.28501037471662</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:6">
@@ -1407,7 +1326,7 @@
         <v>37</v>
       </c>
       <c r="C35">
-        <v>-0.0268756059235731</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1421,13 +1340,13 @@
         <v>38</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>-0.70140490779583</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>-1.05442425662798</v>
       </c>
       <c r="F36">
-        <v>-19.8146122160927</v>
+        <v>-0.0654259315329985</v>
       </c>
     </row>
     <row r="37" spans="2:6">
@@ -1435,13 +1354,13 @@
         <v>39</v>
       </c>
       <c r="C37">
-        <v>0.701404907827371</v>
+        <v>38.2699921375394</v>
       </c>
       <c r="D37">
-        <v>0.0131585445355181</v>
+        <v>5.04574879354213</v>
       </c>
       <c r="F37">
-        <v>1.14077150892348</v>
+        <v>67.1543698105053</v>
       </c>
     </row>
     <row r="38" spans="2:6">
@@ -1449,10 +1368,10 @@
         <v>40</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>-0.0134378029705174</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>-0.0165757920139583</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1463,7 +1382,7 @@
         <v>41</v>
       </c>
       <c r="C39">
-        <v>0.0134378029617868</v>
+        <v>0.280508023475898</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -1477,13 +1396,13 @@
         <v>42</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>0.70140490779583</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1.05442425662798</v>
       </c>
       <c r="F40">
-        <v>19.8146122160927</v>
+        <v>0.0654259315329985</v>
       </c>
     </row>
     <row r="41" spans="2:6">
@@ -1491,13 +1410,13 @@
         <v>43</v>
       </c>
       <c r="C41">
-        <v>-0.701404907827371</v>
+        <v>0.0161936355489839</v>
       </c>
       <c r="D41">
-        <v>-0.0131585445355181</v>
+        <v>-0.088549044361916</v>
       </c>
       <c r="F41">
-        <v>-1.14077150892348</v>
+        <v>2.84563018949468</v>
       </c>
     </row>
     <row r="42" spans="2:6">
@@ -1505,13 +1424,13 @@
         <v>44</v>
       </c>
       <c r="C42">
-        <v>38.2699921423637</v>
+        <v>0.0134378029705174</v>
       </c>
       <c r="D42">
-        <v>15.6989635336133</v>
+        <v>0.0165757920139583</v>
       </c>
       <c r="F42">
-        <v>37.989561905906</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:6">
@@ -1519,7 +1438,7 @@
         <v>45</v>
       </c>
       <c r="C43">
-        <v>-0.0134378029617868</v>
+        <v>0.280508023475898</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1533,13 +1452,13 @@
         <v>46</v>
       </c>
       <c r="C44">
-        <v>0.280508023523387</v>
+        <v>0.70140490779583</v>
       </c>
       <c r="D44">
-        <v>-0.112785799305306</v>
+        <v>1.05442425662798</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>0.0654259315329985</v>
       </c>
     </row>
     <row r="45" spans="2:6">
@@ -1547,13 +1466,13 @@
         <v>47</v>
       </c>
       <c r="C45">
-        <v>0.701404907827371</v>
+        <v>0.0161936355489839</v>
       </c>
       <c r="D45">
-        <v>0.0131585445355178</v>
+        <v>-0.088549044361916</v>
       </c>
       <c r="F45">
-        <v>1.14077150892348</v>
+        <v>2.84563018949468</v>
       </c>
     </row>
     <row r="46" spans="2:6">
@@ -1561,13 +1480,13 @@
         <v>48</v>
       </c>
       <c r="C46">
-        <v>0.0161936355517248</v>
+        <v>0.0134378029705174</v>
       </c>
       <c r="D46">
-        <v>-10.9656323778912</v>
+        <v>0.0165757920139583</v>
       </c>
       <c r="F46">
-        <v>12.1958258780013</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:6">
@@ -1575,7 +1494,7 @@
         <v>49</v>
       </c>
       <c r="C47">
-        <v>0.0134378029617863</v>
+        <v>0.0438318116061436</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1589,13 +1508,13 @@
         <v>50</v>
       </c>
       <c r="C48">
-        <v>0.280508023523387</v>
+        <v>0.70140490779583</v>
       </c>
       <c r="D48">
-        <v>-0.112785799305308</v>
+        <v>1.05442425662798</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>0.0654259315329985</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -1603,13 +1522,13 @@
         <v>51</v>
       </c>
       <c r="C49">
-        <v>0.701404907827371</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>0.0131585445355178</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>1.14077150892348</v>
+        <v>2.82453433127071</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -1617,35 +1536,29 @@
         <v>52</v>
       </c>
       <c r="C50">
-        <v>0.0161936355517248</v>
+        <v>0.0134378029705174</v>
       </c>
       <c r="D50">
-        <v>-10.9656323778912</v>
+        <v>0.0165757920139583</v>
       </c>
       <c r="F50">
-        <v>12.1958258780013</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C51">
-        <v>0.0134378029617863</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>0</v>
+      <c r="C51" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="2:6">
       <c r="B52" s="1" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="C52">
-        <v>0.0438318116135627</v>
+        <v>0</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -1656,21 +1569,21 @@
     </row>
     <row r="53" spans="2:6">
       <c r="B53" s="1" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="C53">
-        <v>0.701404907827372</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>0.0131585445355179</v>
+        <v>0</v>
       </c>
       <c r="F53">
-        <v>1.14077150892348</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:6">
       <c r="B54" s="1" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1679,15 +1592,15 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>12.1958258780013</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:6">
       <c r="B55" s="1" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="C55">
-        <v>0.0134378029617863</v>
+        <v>0</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -1698,10 +1611,16 @@
     </row>
     <row r="56" spans="2:6">
       <c r="B56" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C56" t="s">
-        <v>186</v>
+        <v>17</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>-0.042404065483858</v>
       </c>
     </row>
     <row r="57" spans="2:6">
@@ -1715,7 +1634,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>1.47165233828602</v>
+        <v>-0.042404065483858</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -1723,13 +1642,13 @@
         <v>19</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>-1.2018036174373</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>-1.76919890724782</v>
       </c>
       <c r="F58">
-        <v>0.654712533196115</v>
+        <v>-0.473168200022645</v>
       </c>
     </row>
     <row r="59" spans="2:6">
@@ -1737,13 +1656,13 @@
         <v>20</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>-1.2018036174373</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>-1.76919890724782</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>-0.473168200022645</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -1771,7 +1690,7 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>-4.72531330758772</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -1785,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <v>-4.72531330758772</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -1793,13 +1712,13 @@
         <v>24</v>
       </c>
       <c r="C63">
-        <v>-1.20180361756454</v>
+        <v>0.0268756059410347</v>
       </c>
       <c r="D63">
-        <v>-4.67768415098149</v>
+        <v>0.0264577059376176</v>
       </c>
       <c r="F63">
-        <v>8.46211513547727</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -1807,13 +1726,13 @@
         <v>25</v>
       </c>
       <c r="C64">
-        <v>-1.20180361756454</v>
+        <v>-0.685115350149317</v>
       </c>
       <c r="D64">
-        <v>-4.67768415098149</v>
+        <v>-0.876302734139586</v>
       </c>
       <c r="F64">
-        <v>8.46211513547727</v>
+        <v>-0.124044341583801</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -1821,13 +1740,13 @@
         <v>26</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>0.17127883753733</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>0.300421621460615</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>-0.0654259315329966</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -1835,13 +1754,13 @@
         <v>27</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>-7.79357979984874</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>-1.67109711155474</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>-13.6701065583721</v>
       </c>
     </row>
     <row r="67" spans="2:6">
@@ -1849,10 +1768,10 @@
         <v>28</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>0.0268756059410347</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>0.0264577059376176</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -1863,13 +1782,13 @@
         <v>29</v>
       </c>
       <c r="C68">
-        <v>0.0268756059235726</v>
+        <v>0.685115350149317</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>0.876302734139586</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>0.124044341583801</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -1877,13 +1796,13 @@
         <v>30</v>
       </c>
       <c r="C69">
-        <v>-0.685115350265279</v>
+        <v>-0.198154443478364</v>
       </c>
       <c r="D69">
-        <v>-3.75891089584869</v>
+        <v>-0.300421621460615</v>
       </c>
       <c r="F69">
-        <v>-4.72531330758772</v>
+        <v>0.0654259315329966</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -1891,13 +1810,13 @@
         <v>31</v>
       </c>
       <c r="C70">
-        <v>0.171278837566319</v>
+        <v>14.3772591644857</v>
       </c>
       <c r="D70">
-        <v>-0.186278669032052</v>
+        <v>1.67109711155474</v>
       </c>
       <c r="F70">
-        <v>0.486058975727367</v>
+        <v>26.8564969876096</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -1905,13 +1824,13 @@
         <v>32</v>
       </c>
       <c r="C71">
-        <v>-7.79357980084795</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>-4.20715971820001</v>
+        <v>-0.0264577059376176</v>
       </c>
       <c r="F71">
-        <v>-4.59344042007828</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -1919,7 +1838,7 @@
         <v>33</v>
       </c>
       <c r="C72">
-        <v>0.0268756059235726</v>
+        <v>0</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -1933,13 +1852,13 @@
         <v>34</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>0.70140490779583</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>1.05442425662798</v>
       </c>
       <c r="F73">
-        <v>15.0892989085049</v>
+        <v>0.0654259315329985</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -1947,13 +1866,13 @@
         <v>35</v>
       </c>
       <c r="C74">
-        <v>-0.171278837566319</v>
+        <v>-0.00529407316024472</v>
       </c>
       <c r="D74">
-        <v>0.186278669032051</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>-0.486058975727367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -1961,13 +1880,13 @@
         <v>36</v>
       </c>
       <c r="C75">
-        <v>15.0623745166208</v>
+        <v>0.0134378029705174</v>
       </c>
       <c r="D75">
-        <v>7.96607061404871</v>
+        <v>0.0165757920139583</v>
       </c>
       <c r="F75">
-        <v>7.28501037471662</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -1975,7 +1894,7 @@
         <v>37</v>
       </c>
       <c r="C76">
-        <v>-0.0268756059235731</v>
+        <v>0</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -1989,13 +1908,13 @@
         <v>38</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>-0.70140490779583</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>-1.05442425662798</v>
       </c>
       <c r="F77">
-        <v>-19.8146122160927</v>
+        <v>-0.0654259315329985</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2003,13 +1922,13 @@
         <v>39</v>
       </c>
       <c r="C78">
-        <v>0.701404907827371</v>
+        <v>38.2699921375394</v>
       </c>
       <c r="D78">
-        <v>0.0131585445355181</v>
+        <v>5.04574879354213</v>
       </c>
       <c r="F78">
-        <v>1.14077150892348</v>
+        <v>67.1543698105053</v>
       </c>
     </row>
     <row r="79" spans="2:6">
@@ -2017,10 +1936,10 @@
         <v>40</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>-0.0134378029705174</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>-0.0165757920139583</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -2031,7 +1950,7 @@
         <v>41</v>
       </c>
       <c r="C80">
-        <v>0.0134378029617868</v>
+        <v>0.280508023475898</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -2045,13 +1964,13 @@
         <v>42</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>0.70140490779583</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>1.05442425662798</v>
       </c>
       <c r="F81">
-        <v>19.8146122160927</v>
+        <v>0.0654259315329985</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2059,13 +1978,13 @@
         <v>43</v>
       </c>
       <c r="C82">
-        <v>-0.701404907827371</v>
+        <v>0.0161936355489839</v>
       </c>
       <c r="D82">
-        <v>-0.0131585445355181</v>
+        <v>-0.088549044361916</v>
       </c>
       <c r="F82">
-        <v>-1.14077150892348</v>
+        <v>2.84563018949468</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -2073,13 +1992,13 @@
         <v>44</v>
       </c>
       <c r="C83">
-        <v>38.2699921423637</v>
+        <v>0.0134378029705174</v>
       </c>
       <c r="D83">
-        <v>15.6989635336133</v>
+        <v>0.0165757920139583</v>
       </c>
       <c r="F83">
-        <v>37.989561905906</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2087,7 +2006,7 @@
         <v>45</v>
       </c>
       <c r="C84">
-        <v>-0.0134378029617868</v>
+        <v>0.280508023475898</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -2101,13 +2020,13 @@
         <v>46</v>
       </c>
       <c r="C85">
-        <v>0.280508023523387</v>
+        <v>0.70140490779583</v>
       </c>
       <c r="D85">
-        <v>-0.112785799305306</v>
+        <v>1.05442425662798</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>0.0654259315329985</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2115,13 +2034,13 @@
         <v>47</v>
       </c>
       <c r="C86">
-        <v>0.701404907827371</v>
+        <v>0.0161936355489839</v>
       </c>
       <c r="D86">
-        <v>0.0131585445355178</v>
+        <v>-0.088549044361916</v>
       </c>
       <c r="F86">
-        <v>1.14077150892348</v>
+        <v>2.84563018949468</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2129,13 +2048,13 @@
         <v>48</v>
       </c>
       <c r="C87">
-        <v>0.0161936355517248</v>
+        <v>0.0134378029705174</v>
       </c>
       <c r="D87">
-        <v>-10.9656323778912</v>
+        <v>0.0165757920139583</v>
       </c>
       <c r="F87">
-        <v>12.1958258780013</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -2143,7 +2062,7 @@
         <v>49</v>
       </c>
       <c r="C88">
-        <v>0.0134378029617863</v>
+        <v>0.0438318116061436</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -2157,13 +2076,13 @@
         <v>50</v>
       </c>
       <c r="C89">
-        <v>0.280508023523387</v>
+        <v>0.70140490779583</v>
       </c>
       <c r="D89">
-        <v>-0.112785799305308</v>
+        <v>1.05442425662798</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>0.0654259315329985</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -2171,13 +2090,13 @@
         <v>51</v>
       </c>
       <c r="C90">
-        <v>0.701404907827371</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>0.0131585445355178</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>1.14077150892348</v>
+        <v>2.82453433127071</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -2185,27 +2104,27 @@
         <v>52</v>
       </c>
       <c r="C91">
-        <v>0.0161936355517248</v>
+        <v>0.0134378029705174</v>
       </c>
       <c r="D91">
-        <v>-10.9656323778912</v>
+        <v>0.0165757920139583</v>
       </c>
       <c r="F91">
-        <v>12.1958258780013</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="2:6">
       <c r="B92" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C92">
-        <v>0.0134378029617863</v>
+        <v>-1.2018036174373</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>-1.76919890724782</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>-0.473168200022645</v>
       </c>
     </row>
     <row r="93" spans="2:6">
@@ -2213,52 +2132,52 @@
         <v>54</v>
       </c>
       <c r="C93">
-        <v>0.0438318116135627</v>
+        <v>-0.610192041678203</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>-0.808025081753322</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>-0.392555589197982</v>
       </c>
     </row>
     <row r="94" spans="2:6">
       <c r="B94" s="1" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="C94">
-        <v>0.701404907827372</v>
+        <v>0</v>
       </c>
       <c r="D94">
-        <v>0.0131585445355179</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>1.14077150892348</v>
+        <v>-0.042404065483858</v>
       </c>
     </row>
     <row r="95" spans="2:6">
       <c r="B95" s="1" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>0.17127883753733</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>0.300421621460615</v>
       </c>
       <c r="F95">
-        <v>12.1958258780013</v>
+        <v>-0.130851863065994</v>
       </c>
     </row>
     <row r="96" spans="2:6">
       <c r="B96" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C96">
-        <v>0.0134378029617863</v>
+        <v>0</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>0.0490508978465372</v>
       </c>
       <c r="F96">
         <v>0</v>
@@ -2266,58 +2185,58 @@
     </row>
     <row r="97" spans="2:6">
       <c r="B97" s="1" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C97">
-        <v>-1.20180361756454</v>
+        <v>0.318533823809619</v>
       </c>
       <c r="D97">
-        <v>-4.67768415098149</v>
+        <v>0.41724139384547</v>
       </c>
       <c r="F97">
-        <v>8.46211513547727</v>
+        <v>0.196277794598991</v>
       </c>
     </row>
     <row r="98" spans="2:6">
       <c r="B98" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C98">
-        <v>-0.610192041695173</v>
+        <v>6.58367936463695</v>
       </c>
       <c r="D98">
-        <v>-0.771431765199243</v>
+        <v>-0.0490508978465372</v>
       </c>
       <c r="F98">
-        <v>-0.337307114937497</v>
+        <v>13.1863904292375</v>
       </c>
     </row>
     <row r="99" spans="2:6">
       <c r="B99" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>-0.318533823809619</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>-0.41724139384547</v>
       </c>
       <c r="F99">
-        <v>-4.72531330758772</v>
+        <v>-0.196277794598991</v>
       </c>
     </row>
     <row r="100" spans="2:6">
       <c r="B100" s="1" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="C100">
-        <v>0.17127883756632</v>
+        <v>-6.59177618241144</v>
       </c>
       <c r="D100">
-        <v>-0.186278669032052</v>
+        <v>0.0490508978465374</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>-13.1969383583495</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -2325,13 +2244,13 @@
         <v>60</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>0.318533823809619</v>
       </c>
       <c r="D101">
-        <v>0.242036912587244</v>
+        <v>0.41724139384547</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>0.196277794598991</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -2339,13 +2258,13 @@
         <v>61</v>
       </c>
       <c r="C102">
-        <v>0.318533823809373</v>
+        <v>-13.1754555470484</v>
       </c>
       <c r="D102">
-        <v>0.385715882599621</v>
+        <v>-0.0506736561714556</v>
       </c>
       <c r="F102">
-        <v>0.168653557468749</v>
+        <v>-26.8172607769936</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -2353,13 +2272,13 @@
         <v>62</v>
       </c>
       <c r="C103">
-        <v>6.58367936550754</v>
+        <v>0.0995342151641704</v>
       </c>
       <c r="D103">
-        <v>-0.242036912587244</v>
+        <v>0.00114945354142548</v>
       </c>
       <c r="F103">
-        <v>13.0555555555556</v>
+        <v>0.220388872067676</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -2367,13 +2286,13 @@
         <v>63</v>
       </c>
       <c r="C104">
-        <v>-0.318533823809373</v>
+        <v>0</v>
       </c>
       <c r="D104">
-        <v>-0.385715882599621</v>
+        <v>0.14877545186453</v>
       </c>
       <c r="F104">
-        <v>-0.168653557468749</v>
+        <v>0.43393198940656</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -2381,13 +2300,13 @@
         <v>64</v>
       </c>
       <c r="C105">
-        <v>-6.5917761832834</v>
+        <v>0.537533432455068</v>
       </c>
       <c r="D105">
-        <v>0.228487520194235</v>
+        <v>0.833333334149514</v>
       </c>
       <c r="F105">
-        <v>-13.0555555555556</v>
+        <v>0.172166717130306</v>
       </c>
     </row>
     <row r="106" spans="2:6">
@@ -2395,13 +2314,13 @@
         <v>65</v>
       </c>
       <c r="C106">
-        <v>0.318533823809373</v>
+        <v>6.57963095574971</v>
       </c>
       <c r="D106">
-        <v>0.385715882599621</v>
+        <v>-0.0506736561714556</v>
       </c>
       <c r="F106">
-        <v>0.168653557468749</v>
+        <v>13.1827392230064</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -2409,13 +2328,13 @@
         <v>66</v>
       </c>
       <c r="C107">
-        <v>-13.1754555487909</v>
+        <v>-0.318533823809619</v>
       </c>
       <c r="D107">
-        <v>-0.248811608783751</v>
+        <v>-0.41724139384547</v>
       </c>
       <c r="F107">
-        <v>-26.9444444444444</v>
+        <v>-0.196277794598991</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -2423,13 +2342,13 @@
         <v>67</v>
       </c>
       <c r="C108">
-        <v>0.0995342151646544</v>
+        <v>0</v>
       </c>
       <c r="D108">
-        <v>0.0309507840670452</v>
+        <v>0</v>
       </c>
       <c r="F108">
-        <v>0.248013109197917</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -2440,10 +2359,10 @@
         <v>0</v>
       </c>
       <c r="D109">
-        <v>0.71933604156523</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>0.833333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -2451,13 +2370,13 @@
         <v>69</v>
       </c>
       <c r="C110">
-        <v>0.537533432454092</v>
+        <v>0</v>
       </c>
       <c r="D110">
-        <v>0.740480981132198</v>
+        <v>0</v>
       </c>
       <c r="F110">
-        <v>0.0892940057395797</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -2465,13 +2384,13 @@
         <v>70</v>
       </c>
       <c r="C111">
-        <v>6.57963095661961</v>
+        <v>0.418068038973789</v>
       </c>
       <c r="D111">
-        <v>-0.248811608783751</v>
+        <v>0.418390847386895</v>
       </c>
       <c r="F111">
-        <v>13.0555555555556</v>
+        <v>0.416666666666667</v>
       </c>
     </row>
     <row r="112" spans="2:6">
@@ -2479,13 +2398,13 @@
         <v>71</v>
       </c>
       <c r="C112">
-        <v>-0.318533823809373</v>
+        <v>0</v>
       </c>
       <c r="D112">
-        <v>-0.385715882599621</v>
+        <v>0.14877545186453</v>
       </c>
       <c r="F112">
-        <v>-0.168653557468749</v>
+        <v>0.43393198940656</v>
       </c>
     </row>
     <row r="113" spans="2:6">
@@ -2493,13 +2412,13 @@
         <v>72</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>0.537533432455068</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>0.833333334149514</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>0.172166717130306</v>
       </c>
     </row>
     <row r="114" spans="2:6">
@@ -2521,13 +2440,13 @@
         <v>74</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>0.418068038973789</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>0.418390847386895</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>0.416666666666667</v>
       </c>
     </row>
     <row r="116" spans="2:6">
@@ -2535,13 +2454,13 @@
         <v>75</v>
       </c>
       <c r="C116">
-        <v>0.418068038974027</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>0.416666666666667</v>
+        <v>0.14877545186453</v>
       </c>
       <c r="F116">
-        <v>0.416666666666667</v>
+        <v>0.43393198940656</v>
       </c>
     </row>
     <row r="117" spans="2:6">
@@ -2549,13 +2468,13 @@
         <v>76</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>0.537533432455068</v>
       </c>
       <c r="D117">
-        <v>0.719336041565233</v>
+        <v>0.833333334149514</v>
       </c>
       <c r="F117">
-        <v>0.833333333333333</v>
+        <v>0.172166717130306</v>
       </c>
     </row>
     <row r="118" spans="2:6">
@@ -2563,13 +2482,13 @@
         <v>77</v>
       </c>
       <c r="C118">
-        <v>0.537533432454092</v>
+        <v>0</v>
       </c>
       <c r="D118">
-        <v>0.740480981132198</v>
+        <v>0.14877545186453</v>
       </c>
       <c r="F118">
-        <v>0.0892940057395797</v>
+        <v>0.43393198940656</v>
       </c>
     </row>
     <row r="119" spans="2:6">
@@ -2577,13 +2496,13 @@
         <v>78</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>0.537533432455068</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>0.833333334149514</v>
       </c>
       <c r="F119">
-        <v>0</v>
+        <v>0.172166717130306</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -2591,13 +2510,13 @@
         <v>79</v>
       </c>
       <c r="C120">
-        <v>0.418068038974027</v>
+        <v>0</v>
       </c>
       <c r="D120">
-        <v>0.416666666666667</v>
+        <v>0</v>
       </c>
       <c r="F120">
-        <v>0.416666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="2:6">
@@ -2605,13 +2524,13 @@
         <v>80</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>0.418068038973789</v>
       </c>
       <c r="D121">
-        <v>0.719336041565233</v>
+        <v>0.418390847386895</v>
       </c>
       <c r="F121">
-        <v>0.833333333333333</v>
+        <v>0.416666666666667</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -2619,13 +2538,13 @@
         <v>81</v>
       </c>
       <c r="C122">
-        <v>0.537533432454092</v>
+        <v>4.54993845125947</v>
       </c>
       <c r="D122">
-        <v>0.740480981132198</v>
+        <v>0</v>
       </c>
       <c r="F122">
-        <v>0.0892940057395797</v>
+        <v>21.4321238123358</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -2633,13 +2552,13 @@
         <v>82</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>4.54993845125947</v>
       </c>
       <c r="D123">
-        <v>0.719336041565233</v>
+        <v>0</v>
       </c>
       <c r="F123">
-        <v>0.833333333333333</v>
+        <v>21.4321238123358</v>
       </c>
     </row>
     <row r="124" spans="2:6">
@@ -2647,13 +2566,13 @@
         <v>83</v>
       </c>
       <c r="C124">
-        <v>0.537533432454092</v>
+        <v>0</v>
       </c>
       <c r="D124">
-        <v>0.740480981132198</v>
+        <v>0</v>
       </c>
       <c r="F124">
-        <v>0.0892940057395797</v>
+        <v>2.02572425256996</v>
       </c>
     </row>
     <row r="125" spans="2:6">
@@ -2661,13 +2580,13 @@
         <v>84</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>0.556876910146691</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>0.545921007086394</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>0.729555077055206</v>
       </c>
     </row>
     <row r="126" spans="2:6">
@@ -2675,13 +2594,13 @@
         <v>85</v>
       </c>
       <c r="C126">
-        <v>0.418068038974027</v>
+        <v>2.27496922562973</v>
       </c>
       <c r="D126">
-        <v>0.416666666666667</v>
+        <v>0</v>
       </c>
       <c r="F126">
-        <v>0.416666666666667</v>
+        <v>11.7289240324529</v>
       </c>
     </row>
     <row r="127" spans="2:6">
@@ -2689,13 +2608,13 @@
         <v>86</v>
       </c>
       <c r="C127">
-        <v>4.54993844570634</v>
+        <v>1.59644228913</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>1.37704943948562</v>
       </c>
       <c r="F127">
-        <v>15.0611074065662</v>
+        <v>1.75393142793838</v>
       </c>
     </row>
     <row r="128" spans="2:6">
@@ -2703,13 +2622,13 @@
         <v>87</v>
       </c>
       <c r="C128">
-        <v>4.54993844570634</v>
+        <v>4.54993845125947</v>
       </c>
       <c r="D128">
         <v>0</v>
       </c>
       <c r="F128">
-        <v>15.0611074065662</v>
+        <v>23.4578480649058</v>
       </c>
     </row>
     <row r="129" spans="2:6">
@@ -2717,13 +2636,13 @@
         <v>88</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>3.19288457825999</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>2.75409887897124</v>
       </c>
       <c r="F129">
-        <v>0</v>
+        <v>3.50786285587677</v>
       </c>
     </row>
     <row r="130" spans="2:6">
@@ -2731,74 +2650,74 @@
         <v>89</v>
       </c>
       <c r="C130">
-        <v>0.556876910142766</v>
+        <v>0</v>
       </c>
       <c r="D130">
-        <v>1.08425165497412</v>
+        <v>0</v>
       </c>
       <c r="F130">
-        <v>0.426235603374606</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="2:6">
       <c r="B131" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C131">
-        <v>2.27496922285317</v>
+        <v>0</v>
       </c>
       <c r="D131">
         <v>0</v>
       </c>
       <c r="F131">
-        <v>7.53055370328308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="2:6">
       <c r="B132" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C132">
-        <v>1.59644228915475</v>
+        <v>0</v>
       </c>
       <c r="D132">
-        <v>1.63953602332924</v>
+        <v>0</v>
       </c>
       <c r="F132">
-        <v>1.80846138732092</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="2:6">
       <c r="B133" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C133">
-        <v>4.54993844570634</v>
+        <v>0</v>
       </c>
       <c r="D133">
         <v>0</v>
       </c>
       <c r="F133">
-        <v>15.0611074065662</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="2:6">
       <c r="B134" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C134">
-        <v>3.1928845783095</v>
+        <v>24.25</v>
       </c>
       <c r="D134">
-        <v>3.27907204665848</v>
+        <v>24.25</v>
       </c>
       <c r="F134">
-        <v>3.61692277464184</v>
+        <v>24.25</v>
       </c>
     </row>
     <row r="135" spans="2:6">
       <c r="B135" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2812,21 +2731,21 @@
     </row>
     <row r="136" spans="2:6">
       <c r="B136" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>48.5</v>
       </c>
       <c r="D136">
-        <v>0</v>
+        <v>48.5</v>
       </c>
       <c r="F136">
-        <v>0</v>
+        <v>48.5</v>
       </c>
     </row>
     <row r="137" spans="2:6">
       <c r="B137" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2843,13 +2762,13 @@
         <v>95</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="F138">
-        <v>0</v>
+        <v>97</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -2857,13 +2776,13 @@
         <v>96</v>
       </c>
       <c r="C139">
-        <v>24.25</v>
+        <v>0</v>
       </c>
       <c r="D139">
-        <v>24.25</v>
+        <v>0</v>
       </c>
       <c r="F139">
-        <v>24.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -2871,13 +2790,13 @@
         <v>97</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>44.254219079837</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>41.1694147782276</v>
       </c>
       <c r="F140">
-        <v>0</v>
+        <v>48.5</v>
       </c>
     </row>
     <row r="141" spans="2:6">
@@ -2885,13 +2804,13 @@
         <v>98</v>
       </c>
       <c r="C141">
-        <v>48.5</v>
+        <v>0</v>
       </c>
       <c r="D141">
-        <v>48.5</v>
+        <v>0</v>
       </c>
       <c r="F141">
-        <v>48.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -2913,13 +2832,13 @@
         <v>100</v>
       </c>
       <c r="C143">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="D143">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="F143">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -2927,13 +2846,13 @@
         <v>101</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>-0.513836512611988</v>
       </c>
       <c r="D144">
         <v>0</v>
       </c>
       <c r="F144">
-        <v>0</v>
+        <v>-0.669387809029899</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -2941,13 +2860,13 @@
         <v>102</v>
       </c>
       <c r="C145">
-        <v>44.2542190792098</v>
+        <v>-0.171278837537329</v>
       </c>
       <c r="D145">
-        <v>48.4890562599903</v>
+        <v>0</v>
       </c>
       <c r="F145">
-        <v>38.8604166335585</v>
+        <v>-0.223129269676633</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -2955,13 +2874,13 @@
         <v>103</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>-0.0226555189651649</v>
       </c>
       <c r="D146">
         <v>0</v>
       </c>
       <c r="F146">
-        <v>0</v>
+        <v>-0.0295139170345001</v>
       </c>
     </row>
     <row r="147" spans="2:6">
@@ -2969,13 +2888,13 @@
         <v>104</v>
       </c>
       <c r="C147">
-        <v>0</v>
+        <v>-0.00755183965505497</v>
       </c>
       <c r="D147">
         <v>0</v>
       </c>
       <c r="F147">
-        <v>0</v>
+        <v>-0.00983797234483337</v>
       </c>
     </row>
     <row r="148" spans="2:6">
@@ -2983,13 +2902,13 @@
         <v>105</v>
       </c>
       <c r="C148">
-        <v>0</v>
+        <v>-0.00373699281899627</v>
       </c>
       <c r="D148">
         <v>0</v>
       </c>
       <c r="F148">
-        <v>0</v>
+        <v>-0.00486827497476291</v>
       </c>
     </row>
     <row r="149" spans="2:6">
@@ -2997,13 +2916,13 @@
         <v>106</v>
       </c>
       <c r="C149">
-        <v>-0.513836512698959</v>
+        <v>-0.00124566427299876</v>
       </c>
       <c r="D149">
         <v>0</v>
       </c>
       <c r="F149">
-        <v>-0.859865286479391</v>
+        <v>-0.00162275832492097</v>
       </c>
     </row>
     <row r="150" spans="2:6">
@@ -3011,13 +2930,13 @@
         <v>107</v>
       </c>
       <c r="C150">
-        <v>-0.17127883756632</v>
+        <v>-0.0221883948627904</v>
       </c>
       <c r="D150">
         <v>0</v>
       </c>
       <c r="F150">
-        <v>-0.286621762159797</v>
+        <v>-0.0289053826626548</v>
       </c>
     </row>
     <row r="151" spans="2:6">
@@ -3025,13 +2944,13 @@
         <v>108</v>
       </c>
       <c r="C151">
-        <v>-0.0226555189689996</v>
+        <v>-0.00739613162093012</v>
       </c>
       <c r="D151">
         <v>0</v>
       </c>
       <c r="F151">
-        <v>-0.0379122421765913</v>
+        <v>-0.00963512755421825</v>
       </c>
     </row>
     <row r="152" spans="2:6">
@@ -3039,13 +2958,13 @@
         <v>109</v>
       </c>
       <c r="C152">
-        <v>-0.00755183965633319</v>
+        <v>-0.0266260738353484</v>
       </c>
       <c r="D152">
         <v>0</v>
       </c>
       <c r="F152">
-        <v>-0.0126374140588638</v>
+        <v>-0.0346864591951857</v>
       </c>
     </row>
     <row r="153" spans="2:6">
@@ -3053,13 +2972,13 @@
         <v>110</v>
       </c>
       <c r="C153">
-        <v>-0.00373699281962879</v>
+        <v>-0.00887535794511615</v>
       </c>
       <c r="D153">
         <v>0</v>
       </c>
       <c r="F153">
-        <v>-0.00625356571985011</v>
+        <v>-0.0115621530650619</v>
       </c>
     </row>
     <row r="154" spans="2:6">
@@ -3067,13 +2986,13 @@
         <v>111</v>
       </c>
       <c r="C154">
-        <v>-0.0012456642732096</v>
+        <v>-0.0775426009941727</v>
       </c>
       <c r="D154">
         <v>0</v>
       </c>
       <c r="F154">
-        <v>-0.0020845219066167</v>
+        <v>-0.10101670572633</v>
       </c>
     </row>
     <row r="155" spans="2:6">
@@ -3081,13 +3000,13 @@
         <v>112</v>
       </c>
       <c r="C155">
-        <v>-0.022188394866546</v>
+        <v>-0.0258475336647242</v>
       </c>
       <c r="D155">
         <v>0</v>
       </c>
       <c r="F155">
-        <v>-0.03713054646161</v>
+        <v>-0.0336722352421101</v>
       </c>
     </row>
     <row r="156" spans="2:6">
@@ -3095,13 +3014,13 @@
         <v>113</v>
       </c>
       <c r="C156">
-        <v>-0.00739613162218199</v>
+        <v>-0.00163493435831087</v>
       </c>
       <c r="D156">
         <v>0</v>
       </c>
       <c r="F156">
-        <v>-0.0123768488205367</v>
+        <v>-0.00212987030145877</v>
       </c>
     </row>
     <row r="157" spans="2:6">
@@ -3109,13 +3028,13 @@
         <v>114</v>
       </c>
       <c r="C157">
-        <v>-0.0266260738398552</v>
+        <v>-0.000544978119436957</v>
       </c>
       <c r="D157">
         <v>0</v>
       </c>
       <c r="F157">
-        <v>-0.0445566557539321</v>
+        <v>-0.000709956767152924</v>
       </c>
     </row>
     <row r="158" spans="2:6">
@@ -3123,13 +3042,13 @@
         <v>115</v>
       </c>
       <c r="C158">
-        <v>-0.00887535794661838</v>
+        <v>-0.0179842779414196</v>
       </c>
       <c r="D158">
         <v>0</v>
       </c>
       <c r="F158">
-        <v>-0.014852218584644</v>
+        <v>-0.0234285733160465</v>
       </c>
     </row>
     <row r="159" spans="2:6">
@@ -3137,13 +3056,13 @@
         <v>116</v>
       </c>
       <c r="C159">
-        <v>-0.0775426010072975</v>
+        <v>-0.00599475931380652</v>
       </c>
       <c r="D159">
         <v>0</v>
       </c>
       <c r="F159">
-        <v>-0.12976148868689</v>
+        <v>-0.00780952443868216</v>
       </c>
     </row>
     <row r="160" spans="2:6">
@@ -3151,13 +3070,13 @@
         <v>117</v>
       </c>
       <c r="C160">
-        <v>-0.0258475336690992</v>
+        <v>-0.0014013723071236</v>
       </c>
       <c r="D160">
         <v>0</v>
       </c>
       <c r="F160">
-        <v>-0.0432538295622966</v>
+        <v>-0.00182560311553609</v>
       </c>
     </row>
     <row r="161" spans="2:6">
@@ -3165,13 +3084,13 @@
         <v>118</v>
       </c>
       <c r="C161">
-        <v>-0.0016349343585876</v>
+        <v>-0.000467124102374534</v>
       </c>
       <c r="D161">
         <v>0</v>
       </c>
       <c r="F161">
-        <v>-0.00273593500243442</v>
+        <v>-0.000608534371845363</v>
       </c>
     </row>
     <row r="162" spans="2:6">
@@ -3179,13 +3098,13 @@
         <v>119</v>
       </c>
       <c r="C162">
-        <v>-0.000544978119529199</v>
+        <v>-0.000934248204749068</v>
       </c>
       <c r="D162">
         <v>0</v>
       </c>
       <c r="F162">
-        <v>-0.000911978334144808</v>
+        <v>-0.00121706874369073</v>
       </c>
     </row>
     <row r="163" spans="2:6">
@@ -3193,13 +3112,13 @@
         <v>120</v>
       </c>
       <c r="C163">
-        <v>-0.0179842779444636</v>
+        <v>-0.000311416068249689</v>
       </c>
       <c r="D163">
         <v>0</v>
       </c>
       <c r="F163">
-        <v>-0.0300952850267787</v>
+        <v>-0.000405689581230242</v>
       </c>
     </row>
     <row r="164" spans="2:6">
@@ -3207,13 +3126,13 @@
         <v>121</v>
       </c>
       <c r="C164">
-        <v>-0.00599475931482119</v>
+        <v>-0.0028027446142472</v>
       </c>
       <c r="D164">
         <v>0</v>
       </c>
       <c r="F164">
-        <v>-0.0100317616755929</v>
+        <v>-0.00365120623107218</v>
       </c>
     </row>
     <row r="165" spans="2:6">
@@ -3221,13 +3140,13 @@
         <v>122</v>
       </c>
       <c r="C165">
-        <v>-0.0014013723073608</v>
+        <v>-0.000934248204749068</v>
       </c>
       <c r="D165">
         <v>0</v>
       </c>
       <c r="F165">
-        <v>-0.00234508714494379</v>
+        <v>-0.00121706874369073</v>
       </c>
     </row>
     <row r="166" spans="2:6">
@@ -3235,13 +3154,13 @@
         <v>123</v>
       </c>
       <c r="C166">
-        <v>-0.000467124102453599</v>
+        <v>-0.0028027446142472</v>
       </c>
       <c r="D166">
         <v>0</v>
       </c>
       <c r="F166">
-        <v>-0.000781695714981264</v>
+        <v>-0.00365120623107218</v>
       </c>
     </row>
     <row r="167" spans="2:6">
@@ -3249,13 +3168,13 @@
         <v>124</v>
       </c>
       <c r="C167">
-        <v>-0.000934248204907198</v>
+        <v>-0.000934248204749068</v>
       </c>
       <c r="D167">
         <v>0</v>
       </c>
       <c r="F167">
-        <v>-0.00156339142996253</v>
+        <v>-0.00121706874369073</v>
       </c>
     </row>
     <row r="168" spans="2:6">
@@ -3263,13 +3182,13 @@
         <v>125</v>
       </c>
       <c r="C168">
-        <v>-0.0003114160683024</v>
+        <v>-0.00420411692137081</v>
       </c>
       <c r="D168">
         <v>0</v>
       </c>
       <c r="F168">
-        <v>-0.000521130476654176</v>
+        <v>-0.00547680934660827</v>
       </c>
     </row>
     <row r="169" spans="2:6">
@@ -3277,13 +3196,13 @@
         <v>126</v>
       </c>
       <c r="C169">
-        <v>-0.0028027446147216</v>
+        <v>-0.0014013723071236</v>
       </c>
       <c r="D169">
         <v>0</v>
       </c>
       <c r="F169">
-        <v>-0.00469017428988758</v>
+        <v>-0.00182560311553609</v>
       </c>
     </row>
     <row r="170" spans="2:6">
@@ -3291,13 +3210,13 @@
         <v>127</v>
       </c>
       <c r="C170">
-        <v>-0.000934248204907198</v>
+        <v>-0.00163493435831087</v>
       </c>
       <c r="D170">
         <v>0</v>
       </c>
       <c r="F170">
-        <v>-0.00156339142996253</v>
+        <v>-0.00212987030145877</v>
       </c>
     </row>
     <row r="171" spans="2:6">
@@ -3305,13 +3224,13 @@
         <v>128</v>
       </c>
       <c r="C171">
-        <v>-0.0028027446147216</v>
+        <v>-0.000544978119436957</v>
       </c>
       <c r="D171">
         <v>0</v>
       </c>
       <c r="F171">
-        <v>-0.00469017428988758</v>
+        <v>-0.000709956767152924</v>
       </c>
     </row>
     <row r="172" spans="2:6">
@@ -3319,13 +3238,13 @@
         <v>129</v>
       </c>
       <c r="C172">
-        <v>-0.000934248204907198</v>
+        <v>-0.00256918256305994</v>
       </c>
       <c r="D172">
         <v>0</v>
       </c>
       <c r="F172">
-        <v>-0.00156339142996253</v>
+        <v>-0.0033469390451495</v>
       </c>
     </row>
     <row r="173" spans="2:6">
@@ -3333,13 +3252,13 @@
         <v>130</v>
       </c>
       <c r="C173">
-        <v>-0.00420411692208239</v>
+        <v>-0.000856394187686646</v>
       </c>
       <c r="D173">
         <v>0</v>
       </c>
       <c r="F173">
-        <v>-0.00703526143483138</v>
+        <v>-0.00111564634838317</v>
       </c>
     </row>
     <row r="174" spans="2:6">
@@ -3347,13 +3266,13 @@
         <v>131</v>
       </c>
       <c r="C174">
-        <v>-0.0014013723073608</v>
+        <v>-0.013079474866487</v>
       </c>
       <c r="D174">
         <v>0</v>
       </c>
       <c r="F174">
-        <v>-0.00234508714494379</v>
+        <v>-0.0170389624116702</v>
       </c>
     </row>
     <row r="175" spans="2:6">
@@ -3361,13 +3280,13 @@
         <v>132</v>
       </c>
       <c r="C175">
-        <v>-0.0016349343585876</v>
+        <v>-0.00435982495549565</v>
       </c>
       <c r="D175">
         <v>0</v>
       </c>
       <c r="F175">
-        <v>-0.00273593500243442</v>
+        <v>-0.00567965413722339</v>
       </c>
     </row>
     <row r="176" spans="2:6">
@@ -3375,13 +3294,13 @@
         <v>133</v>
       </c>
       <c r="C176">
-        <v>-0.000544978119529199</v>
+        <v>-0.0021020584606854</v>
       </c>
       <c r="D176">
         <v>0</v>
       </c>
       <c r="F176">
-        <v>-0.000911978334144808</v>
+        <v>-0.00273840467330413</v>
       </c>
     </row>
     <row r="177" spans="2:6">
@@ -3389,13 +3308,13 @@
         <v>134</v>
       </c>
       <c r="C177">
-        <v>-0.0025691825634948</v>
+        <v>-0.000700686153561801</v>
       </c>
       <c r="D177">
         <v>0</v>
       </c>
       <c r="F177">
-        <v>-0.00429932643239695</v>
+        <v>-0.000912801557768045</v>
       </c>
     </row>
     <row r="178" spans="2:6">
@@ -3403,13 +3322,13 @@
         <v>135</v>
       </c>
       <c r="C178">
-        <v>-0.000856394187831599</v>
+        <v>-0.00560548922849441</v>
       </c>
       <c r="D178">
         <v>0</v>
       </c>
       <c r="F178">
-        <v>-0.00143310881079898</v>
+        <v>-0.00730241246214436</v>
       </c>
     </row>
     <row r="179" spans="2:6">
@@ -3417,13 +3336,13 @@
         <v>136</v>
       </c>
       <c r="C179">
-        <v>-0.0130794748687008</v>
+        <v>-0.00186849640949814</v>
       </c>
       <c r="D179">
         <v>0</v>
       </c>
       <c r="F179">
-        <v>-0.0218874800194754</v>
+        <v>-0.00243413748738145</v>
       </c>
     </row>
     <row r="180" spans="2:6">
@@ -3431,13 +3350,13 @@
         <v>137</v>
       </c>
       <c r="C180">
-        <v>-0.00435982495623359</v>
+        <v>12.4547568778803</v>
       </c>
       <c r="D180">
-        <v>0</v>
+        <v>16.3951501260059</v>
       </c>
       <c r="F180">
-        <v>-0.00729582667315846</v>
+        <v>1.85450089839881</v>
       </c>
     </row>
     <row r="181" spans="2:6">
@@ -3445,13 +3364,13 @@
         <v>138</v>
       </c>
       <c r="C181">
-        <v>-0.0021020584610412</v>
+        <v>-2.81549531734768</v>
       </c>
       <c r="D181">
-        <v>0</v>
+        <v>-1.79784803014869</v>
       </c>
       <c r="F181">
-        <v>-0.00351763071741569</v>
+        <v>-3.89449338643638</v>
       </c>
     </row>
     <row r="182" spans="2:6">
@@ -3459,13 +3378,13 @@
         <v>139</v>
       </c>
       <c r="C182">
-        <v>-0.000700686153680399</v>
+        <v>-13.316873335821</v>
       </c>
       <c r="D182">
-        <v>0</v>
+        <v>-23</v>
       </c>
       <c r="F182">
-        <v>-0.0011725435724719</v>
+        <v>3.72892403245289</v>
       </c>
     </row>
     <row r="183" spans="2:6">
@@ -3473,304 +3392,274 @@
         <v>140</v>
       </c>
       <c r="C183">
-        <v>-0.00560548922944319</v>
+        <v>2.84644228912999</v>
       </c>
       <c r="D183">
-        <v>0</v>
+        <v>2.62704943948562</v>
       </c>
       <c r="F183">
-        <v>-0.00938034857977517</v>
+        <v>3.00393142793838</v>
       </c>
     </row>
     <row r="184" spans="2:6">
       <c r="B184" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C184">
-        <v>-0.0018684964098144</v>
-      </c>
-      <c r="D184">
-        <v>0</v>
-      </c>
-      <c r="F184">
-        <v>-0.00312678285992506</v>
+        <v>4</v>
+      </c>
+      <c r="E184">
+        <v>32</v>
       </c>
     </row>
     <row r="185" spans="2:6">
       <c r="B185" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C185">
-        <v>12.4547568795313</v>
-      </c>
-      <c r="D185">
-        <v>-3.14309056486206</v>
-      </c>
-      <c r="F185">
-        <v>25.4738144566141</v>
+        <v>5</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="2:6">
       <c r="B186" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C186">
-        <v>-2.8154953173672</v>
-      </c>
-      <c r="D186">
-        <v>-2.44026254437586</v>
-      </c>
-      <c r="F186">
-        <v>-3.75990970349946</v>
+        <v>6</v>
+      </c>
+      <c r="E186">
+        <v>-43.8942882190986</v>
       </c>
     </row>
     <row r="187" spans="2:6">
       <c r="B187" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C187">
-        <v>-13.3168733376179</v>
-      </c>
-      <c r="D187">
-        <v>-23</v>
-      </c>
-      <c r="F187">
-        <v>-0.46944629671692</v>
+        <v>7</v>
+      </c>
+      <c r="E187">
+        <v>1.11978422241723</v>
       </c>
     </row>
     <row r="188" spans="2:6">
       <c r="B188" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C188">
-        <v>2.84644228915475</v>
-      </c>
-      <c r="D188">
-        <v>2.88953602332924</v>
-      </c>
-      <c r="F188">
-        <v>3.05846138732092</v>
+        <v>8</v>
+      </c>
+      <c r="E188">
+        <v>0.587747532929956</v>
       </c>
     </row>
     <row r="189" spans="2:6">
       <c r="B189" s="1" t="s">
-        <v>146</v>
+        <v>9</v>
       </c>
       <c r="E189">
-        <v>32</v>
+        <v>0.28855520120963</v>
       </c>
     </row>
     <row r="190" spans="2:6">
       <c r="B190" s="1" t="s">
-        <v>147</v>
+        <v>10</v>
       </c>
       <c r="E190">
-        <v>0</v>
+        <v>-1.99837724167508</v>
       </c>
     </row>
     <row r="191" spans="2:6">
       <c r="B191" s="1" t="s">
-        <v>148</v>
+        <v>11</v>
       </c>
       <c r="E191">
-        <v>-46.9044564393636</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="2:6">
       <c r="B192" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E192">
-        <v>0.198863263607615</v>
+        <v>0.00212987030145877</v>
       </c>
     </row>
     <row r="193" spans="2:5">
       <c r="B193" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E193">
-        <v>3.95834810941626</v>
+        <v>0.000709956767152924</v>
       </c>
     </row>
     <row r="194" spans="2:5">
       <c r="B194" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E194">
-        <v>-0.19943721356757</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="2:5">
       <c r="B195" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E195">
-        <v>-2.64373945182588</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="2:5">
       <c r="B196" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E196">
-        <v>-0.0263170890710359</v>
+        <v>0.00162275832492087</v>
       </c>
     </row>
     <row r="197" spans="2:5">
       <c r="B197" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E197">
-        <v>0.00364791333657923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="2:5">
       <c r="B198" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E198">
-        <v>0</v>
+        <v>0.0146048249242887</v>
       </c>
     </row>
     <row r="199" spans="2:5">
       <c r="B199" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E199">
-        <v>0.00469017428988758</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="2:5">
       <c r="B200" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E200">
-        <v>0.00156339142996253</v>
+        <v>0.00365120623107218</v>
       </c>
     </row>
     <row r="201" spans="2:5">
       <c r="B201" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E201">
-        <v>0.00156339142996253</v>
+        <v>0.00121706874369073</v>
       </c>
     </row>
     <row r="202" spans="2:5">
       <c r="B202" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E202">
-        <v>0.000521130476654176</v>
+        <v>21.9678491006875</v>
       </c>
     </row>
     <row r="203" spans="2:5">
       <c r="B203" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="E203">
-        <v>-0.00625356571985011</v>
+        <v>0.0783995115727449</v>
       </c>
     </row>
     <row r="204" spans="2:5">
       <c r="B204" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E204">
-        <v>0</v>
+        <v>-13.1294546428258</v>
       </c>
     </row>
     <row r="205" spans="2:5">
       <c r="B205" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E205">
-        <v>0.00625356571985011</v>
+        <v>0.533851743677157</v>
       </c>
     </row>
     <row r="206" spans="2:5">
       <c r="B206" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E206">
-        <v>0</v>
+        <v>-3.96450216164235</v>
       </c>
     </row>
     <row r="207" spans="2:5">
       <c r="B207" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E207">
-        <v>34.7934445464377</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="2:5">
       <c r="B208" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E208">
-        <v>-0.132679685737622</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209" spans="2:5">
       <c r="B209" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E209">
-        <v>-31.9534891049586</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="2:5">
       <c r="B210" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E210">
-        <v>1.07109311777351</v>
+        <v>0.00547680934660827</v>
       </c>
     </row>
     <row r="211" spans="2:5">
       <c r="B211" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E211">
-        <v>-3.63461587928644</v>
+        <v>0.00182560311553609</v>
       </c>
     </row>
     <row r="212" spans="2:5">
       <c r="B212" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E212">
-        <v>0.0131585445355179</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="2:5">
       <c r="B213" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E213">
-        <v>0.00234508714494379</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="2:5">
       <c r="B214" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E214">
-        <v>0.000781695714981264</v>
+        <v>0.00486827497476291</v>
       </c>
     </row>
     <row r="215" spans="2:5">
       <c r="B215" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E215">
-        <v>0</v>
+        <v>0.00162275832492097</v>
       </c>
     </row>
     <row r="216" spans="2:5">
       <c r="B216" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E216">
         <v>0</v>
@@ -3778,98 +3667,58 @@
     </row>
     <row r="217" spans="2:5">
       <c r="B217" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="E217">
-        <v>0.00429932643239695</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218" spans="2:5">
       <c r="B218" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E218">
-        <v>0.00143310881079898</v>
+        <v>5.25734828330868</v>
       </c>
     </row>
     <row r="219" spans="2:5">
       <c r="B219" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E219">
-        <v>0.00833808762646682</v>
+        <v>-0.581216002285788</v>
       </c>
     </row>
     <row r="220" spans="2:5">
       <c r="B220" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E220">
-        <v>0</v>
+        <v>0.0307309857781908</v>
       </c>
     </row>
     <row r="221" spans="2:5">
       <c r="B221" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E221">
-        <v>0.00351763071741569</v>
+        <v>0.0102436619260636</v>
       </c>
     </row>
     <row r="222" spans="2:5">
       <c r="B222" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="E222">
-        <v>0.0011725435724719</v>
+        <v>0.0170389624116702</v>
       </c>
     </row>
     <row r="223" spans="2:5">
       <c r="B223" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E223">
-        <v>-2.77434937975664</v>
-      </c>
-    </row>
-    <row r="224" spans="2:5">
-      <c r="B224" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E224">
-        <v>-0.898546950571846</v>
-      </c>
-    </row>
-    <row r="225" spans="2:5">
-      <c r="B225" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E225">
-        <v>0.0394756336065538</v>
-      </c>
-    </row>
-    <row r="226" spans="2:5">
-      <c r="B226" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E226">
-        <v>0.0131585445355179</v>
-      </c>
-    </row>
-    <row r="227" spans="2:5">
-      <c r="B227" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E227">
-        <v>0.0291833066926339</v>
-      </c>
-    </row>
-    <row r="228" spans="2:5">
-      <c r="B228" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E228">
-        <v>0</v>
+        <v>0.00567965413722339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving this for future reference
</commit_message>
<xml_diff>
--- a/panda_test.xlsx
+++ b/panda_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="245">
   <si>
     <t>M</t>
   </si>
@@ -28,6 +28,30 @@
     <t>M2</t>
   </si>
   <si>
+    <t>Photon_Light_tx</t>
+  </si>
+  <si>
+    <t>Photon_Dark_tx</t>
+  </si>
+  <si>
+    <t>Suc_Lt_biomass</t>
+  </si>
+  <si>
+    <t>Suc_Dk_biomass</t>
+  </si>
+  <si>
+    <t>CO2_Lt_tx</t>
+  </si>
+  <si>
+    <t>CO2_Dk_tx</t>
+  </si>
+  <si>
+    <t>O2_Lt_tx</t>
+  </si>
+  <si>
+    <t>O2_Dk_tx</t>
+  </si>
+  <si>
     <t>PEPCase_Lt_c</t>
   </si>
   <si>
@@ -46,70 +70,88 @@
     <t>PPDK_Dk_c</t>
   </si>
   <si>
+    <t>CA_Lt_c</t>
+  </si>
+  <si>
+    <t>CA_Dk_c</t>
+  </si>
+  <si>
+    <t>GLY-DC_Lt_m</t>
+  </si>
+  <si>
+    <t>GLY-DC_Dk_m</t>
+  </si>
+  <si>
+    <t>NADP-OAA-to-MAL_Lt_p</t>
+  </si>
+  <si>
+    <t>NADP-OAA-to-MAL_Dk_p</t>
+  </si>
+  <si>
+    <t>NAD-OAA-to-MAL_Lt_p</t>
+  </si>
+  <si>
+    <t>NAD-OAA-to-MAL_Dk_p</t>
+  </si>
+  <si>
+    <t>NAD-OAA-to-MAL_Lt_c</t>
+  </si>
+  <si>
+    <t>NAD-OAA-to-MAL_Dk_c</t>
+  </si>
+  <si>
+    <t>ASP-AT_Lt_p</t>
+  </si>
+  <si>
+    <t>ASP-AT_Dk_p</t>
+  </si>
+  <si>
+    <t>ASP-AT_Lt_c</t>
+  </si>
+  <si>
+    <t>ASP-AT_Dk_c</t>
+  </si>
+  <si>
+    <t>NADP-ME_Lt_p</t>
+  </si>
+  <si>
+    <t>NADP-ME_Dk_p</t>
+  </si>
+  <si>
+    <t>NADP-ME_Lt_c</t>
+  </si>
+  <si>
+    <t>NADP-ME_Dk_c</t>
+  </si>
+  <si>
+    <t>Rubisco-Carbox_Lt_p</t>
+  </si>
+  <si>
+    <t>Rubisco-Carbox_Dk_p</t>
+  </si>
+  <si>
+    <t>Rubisco-Oxy_Lt_p</t>
+  </si>
+  <si>
+    <t>Rubisco-Oxy_Dk_p</t>
+  </si>
+  <si>
     <t>PEP_p_to_c_Lt</t>
   </si>
   <si>
     <t>PEP_p_to_c_Dk</t>
   </si>
   <si>
-    <t>OAA_p_to_c_Lt</t>
-  </si>
-  <si>
-    <t>OAA_p_to_c_Dk</t>
-  </si>
-  <si>
-    <t>NADP-OAA-to-MAL_Lt_p</t>
-  </si>
-  <si>
-    <t>NADP-OAA-to-MAL_Dk_p</t>
-  </si>
-  <si>
-    <t>NAD-OAA-to-MAL_Lt_p</t>
-  </si>
-  <si>
-    <t>NAD-OAA-to-MAL_Dk_p</t>
-  </si>
-  <si>
-    <t>NAD-OAA-to-MAL_Lt_c</t>
-  </si>
-  <si>
-    <t>NAD-OAA-to-MAL_Dk_c</t>
-  </si>
-  <si>
-    <t>ASP-AT_Lt_p</t>
-  </si>
-  <si>
-    <t>ASP-AT_Dk_p</t>
-  </si>
-  <si>
-    <t>ASP-AT_Lt_c</t>
-  </si>
-  <si>
-    <t>ASP-AT_Dk_c</t>
-  </si>
-  <si>
-    <t>NADP-ME_Lt_p</t>
-  </si>
-  <si>
-    <t>NADP-ME_Dk_p</t>
-  </si>
-  <si>
-    <t>NADP-ME_Lt_c</t>
-  </si>
-  <si>
-    <t>NADP-ME_Dk_c</t>
-  </si>
-  <si>
-    <t>Rubisco-Carbox_Lt_p</t>
-  </si>
-  <si>
-    <t>Rubisco-Carbox_Dk_p</t>
-  </si>
-  <si>
-    <t>Rubisco-Oxy_Lt_p</t>
-  </si>
-  <si>
-    <t>Rubisco-Oxy_Dk_p</t>
+    <t>OAA_MAL_Lt_pc</t>
+  </si>
+  <si>
+    <t>OAA_MAL_Dk_pc</t>
+  </si>
+  <si>
+    <t>DHAP_3PGA_Lt_pc</t>
+  </si>
+  <si>
+    <t>DHAP_3PGA_Dk_pc</t>
   </si>
   <si>
     <t>Malate_Lt_M1M2</t>
@@ -124,6 +166,18 @@
     <t>Pyruvate_Dk_M1M2</t>
   </si>
   <si>
+    <t>DHAP_Lt_M1M2</t>
+  </si>
+  <si>
+    <t>DHAP_Dk_M1M2</t>
+  </si>
+  <si>
+    <t>G3P_Lt_M1M2</t>
+  </si>
+  <si>
+    <t>G3p_Dk_M1M2</t>
+  </si>
+  <si>
     <t>Sucrose_Light_M1M2</t>
   </si>
   <si>
@@ -136,6 +190,12 @@
     <t>GLY_Dark_M1M2</t>
   </si>
   <si>
+    <t>CO2_Light_M1M2</t>
+  </si>
+  <si>
+    <t>CO2_Dark_M1M2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hexokinase_Lt_c </t>
   </si>
   <si>
@@ -593,18 +653,6 @@
   </si>
   <si>
     <t>Valine_Dark_biomass</t>
-  </si>
-  <si>
-    <t>CO2_Light_tx</t>
-  </si>
-  <si>
-    <t>CO2_Dark_tx</t>
-  </si>
-  <si>
-    <t>O2_Light_tx</t>
-  </si>
-  <si>
-    <t>O2_Dark_tx</t>
   </si>
   <si>
     <t>MET_Light_M1M2</t>
@@ -1058,7 +1106,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F235"/>
+  <dimension ref="B1:F251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1083,13 +1131,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0.236676211894346</v>
+        <v>290.953536662401</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>185.65505674499</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>185.65505674499</v>
       </c>
     </row>
     <row r="3" spans="2:6">
@@ -1111,13 +1159,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-0.513836512652</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-0.513836512652</v>
       </c>
     </row>
     <row r="5" spans="2:6">
@@ -1125,13 +1173,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-0.171278837550667</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>-0.171278837550667</v>
       </c>
     </row>
     <row r="6" spans="2:6">
@@ -1139,13 +1187,13 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>12.3332705483155</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>15.1744508252917</v>
       </c>
       <c r="F6">
-        <v>0.0135080443705192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:6">
@@ -1153,10 +1201,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>-2.6940089870323</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>-5.53518926400828</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1167,13 +1215,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>-13.3608657196024</v>
       </c>
       <c r="D8">
-        <v>0.981579939494747</v>
+        <v>-19.3103438059023</v>
       </c>
       <c r="F8">
-        <v>-0.0135080443705192</v>
+        <v>3.2709737779883</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -1181,13 +1229,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2.89043467209609</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2.78454403799362</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>2.78439494241387</v>
       </c>
     </row>
     <row r="10" spans="2:6">
@@ -1195,13 +1243,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.202186882326852</v>
       </c>
       <c r="D10">
-        <v>-0.142601968411504</v>
+        <v>20.185038971613</v>
       </c>
       <c r="F10">
-        <v>-1.19049412572518</v>
+        <v>30.0516372402752</v>
       </c>
     </row>
     <row r="11" spans="2:6">
@@ -1209,7 +1257,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.0571448457914956</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1223,13 +1271,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>5.06182861008946</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>7.96470373646306</v>
+        <v>0.868034561220472</v>
       </c>
       <c r="F12">
-        <v>3.76923654874111</v>
+        <v>9.5435746080463</v>
       </c>
     </row>
     <row r="13" spans="2:6">
@@ -1251,13 +1299,13 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>-0.00529407316079467</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>20.1850389716129</v>
       </c>
       <c r="F14">
-        <v>-0.0104380342863105</v>
+        <v>19.2843909151499</v>
       </c>
     </row>
     <row r="15" spans="2:6">
@@ -1265,13 +1313,13 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>-0.0153062993748519</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>-0.0747805001279282</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:6">
@@ -1279,13 +1327,13 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.470861095242467</v>
+        <v>0.202186882326852</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>20.185038971613</v>
       </c>
       <c r="F16">
-        <v>0.552056282648184</v>
+        <v>30.0516372402752</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -1293,13 +1341,13 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>-0.701404907815189</v>
+        <v>0.0571448457914956</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>-1.35840763547731</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -1307,13 +1355,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.00498265709250871</v>
+        <v>6.14625698519007</v>
       </c>
       <c r="D18">
-        <v>-0.142601968411504</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>-0.180670093455694</v>
+        <v>2.14880455316754</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -1327,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.00599475931427637</v>
       </c>
     </row>
     <row r="20" spans="2:6">
@@ -1335,13 +1383,13 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>-0.168943217043014</v>
+        <v>8.00076885206281</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>25.0049826570924</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>51.473601596569</v>
       </c>
     </row>
     <row r="21" spans="2:6">
@@ -1349,13 +1397,13 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>0.0649302502368052</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>0.412737687639377</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>-0.449960217429048</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:6">
@@ -1369,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:6">
@@ -1377,13 +1425,13 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>-0.0327104875997666</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>-0.0644289032559983</v>
       </c>
     </row>
     <row r="24" spans="2:6">
@@ -1391,10 +1439,10 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1.35815460603964</v>
       </c>
       <c r="D24">
-        <v>0.099928828241</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1405,13 +1453,13 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>-0.732272158230353</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>-0.613817615197493</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>-0.552894781801512</v>
       </c>
     </row>
     <row r="26" spans="2:6">
@@ -1419,13 +1467,13 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>14.8163148783012</v>
+        <v>0.00498265709238303</v>
       </c>
       <c r="D26">
-        <v>13.9656365917003</v>
+        <v>0.00498265709238277</v>
       </c>
       <c r="F26">
-        <v>15.3496762312969</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="2:6">
@@ -1447,13 +1495,13 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>4.9387716261004</v>
+        <v>-0.190430925749516</v>
       </c>
       <c r="D28">
-        <v>4.65521219723342</v>
+        <v>-0.478115546055828</v>
       </c>
       <c r="F28">
-        <v>5.11655874376563</v>
+        <v>-47.4960892448</v>
       </c>
     </row>
     <row r="29" spans="2:6">
@@ -1467,22 +1515,34 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>-0.00739613456638858</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E30">
-        <v>1.16839005311886</v>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E31">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="F31">
         <v>0</v>
       </c>
     </row>
@@ -1490,47 +1550,83 @@
       <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E32">
-        <v>-0.715992023133687</v>
+      <c r="C32">
+        <v>0.0226555189669291</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E33">
-        <v>-1.24607102213646</v>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E34">
-        <v>1.01310332778894</v>
+      <c r="C34">
+        <v>18.4323479991621</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>17.2222008643043</v>
       </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E35">
-        <v>-0.00813016611111095</v>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E36">
-        <v>2.65521219723342</v>
+      <c r="C36">
+        <v>12.2882319994414</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>4.30555021607607</v>
       </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E37">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="F37">
         <v>0</v>
       </c>
     </row>
@@ -1545,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>9.53983761522701</v>
       </c>
     </row>
     <row r="39" spans="2:6">
@@ -1567,13 +1663,13 @@
         <v>42</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>-7.99578619497043</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>-1.47360159656903</v>
       </c>
     </row>
     <row r="41" spans="2:6">
@@ -1581,13 +1677,13 @@
         <v>43</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>-0.0327104875997666</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>-0.0644289032559983</v>
       </c>
     </row>
     <row r="42" spans="2:6">
@@ -1601,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>-13.1357348828023</v>
       </c>
     </row>
     <row r="43" spans="2:6">
@@ -1622,55 +1718,31 @@
       <c r="B44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C44">
-        <v>-1.20180361751539</v>
-      </c>
-      <c r="D44">
-        <v>-1.09649645075465</v>
-      </c>
-      <c r="F44">
-        <v>-1.28731114745042</v>
+      <c r="E44">
+        <v>17.5944766983606</v>
       </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C45">
-        <v>-1.20180361751539</v>
-      </c>
-      <c r="D45">
-        <v>-1.09649645075465</v>
-      </c>
-      <c r="F45">
-        <v>-1.28731114745042</v>
+      <c r="E45">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
+      <c r="E46">
+        <v>-21.0574333577892</v>
       </c>
     </row>
     <row r="47" spans="2:6">
       <c r="B47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="F47">
+      <c r="E47">
         <v>0</v>
       </c>
     </row>
@@ -1678,97 +1750,55 @@
       <c r="B48" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
+      <c r="E48">
+        <v>13.4645958433675</v>
       </c>
     </row>
     <row r="49" spans="2:6">
       <c r="B49" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C49">
-        <v>0.0268756059303194</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>0.142192976053755</v>
+      <c r="E49">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:6">
       <c r="B50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C50">
-        <v>-0.685115350220484</v>
-      </c>
-      <c r="D50">
-        <v>-1.00497316167782</v>
-      </c>
-      <c r="F50">
-        <v>-0.345831275374092</v>
+      <c r="E50">
+        <v>-13.4645958433675</v>
       </c>
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C51">
-        <v>0.171278837555121</v>
-      </c>
-      <c r="D51">
-        <v>-0.091523289076804</v>
-      </c>
-      <c r="F51">
-        <v>0.345831275374102</v>
+      <c r="E51">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:6">
       <c r="B52" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C52">
-        <v>-7.79357980046204</v>
-      </c>
-      <c r="D52">
-        <v>-7.31142807328481</v>
-      </c>
-      <c r="F52">
-        <v>-8.11471082328389</v>
+      <c r="E52">
+        <v>0.360181980045458</v>
       </c>
     </row>
     <row r="53" spans="2:6">
       <c r="B53" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C53">
-        <v>0.0268756059303194</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>0.142192976053755</v>
+      <c r="E53">
+        <v>0.149726942198534</v>
       </c>
     </row>
     <row r="54" spans="2:6">
       <c r="B54" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="F54">
+      <c r="E54">
         <v>0</v>
       </c>
     </row>
@@ -1776,42 +1806,24 @@
       <c r="B55" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C55">
-        <v>-0.171278837555121</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>-0.345831275374102</v>
+      <c r="E55">
+        <v>0.00217991247791405</v>
       </c>
     </row>
     <row r="56" spans="2:6">
       <c r="B56" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C56">
-        <v>15.0623745158538</v>
-      </c>
-      <c r="D56">
-        <v>14.5221228272402</v>
-      </c>
-      <c r="F56">
-        <v>15.2811877523062</v>
+      <c r="E56">
+        <v>-5</v>
       </c>
     </row>
     <row r="57" spans="2:6">
       <c r="B57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C57">
-        <v>-0.0268756059303193</v>
-      </c>
-      <c r="D57">
-        <v>0.091523289076804</v>
-      </c>
-      <c r="F57">
-        <v>-0.142192976053755</v>
+      <c r="E57">
+        <v>-2.75064522601469</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -1822,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="D58">
-        <v>0.376314766816554</v>
+        <v>0</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -1833,13 +1845,13 @@
         <v>61</v>
       </c>
       <c r="C59">
-        <v>0.701404907815189</v>
+        <v>0</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
       <c r="F59">
-        <v>1.35840763547731</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -1850,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>-0.00368401210105069</v>
+        <v>0</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -1861,13 +1873,13 @@
         <v>63</v>
       </c>
       <c r="C61">
-        <v>0.0134378029651597</v>
+        <v>0</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
       <c r="F61">
-        <v>0.0710964880268777</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -1878,10 +1890,10 @@
         <v>0</v>
       </c>
       <c r="D62">
-        <v>-0.376314766816554</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>-0.153654532606541</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -1889,13 +1901,13 @@
         <v>65</v>
       </c>
       <c r="C63">
-        <v>-0.701404907815189</v>
+        <v>0</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="F63">
-        <v>-1.35840763547731</v>
+        <v>-0.153654532606541</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -1903,13 +1915,13 @@
         <v>66</v>
       </c>
       <c r="C64">
-        <v>38.2699921405004</v>
+        <v>-1.22484272926519</v>
       </c>
       <c r="D64">
-        <v>37.1967038629374</v>
+        <v>-0.973999595242953</v>
       </c>
       <c r="F64">
-        <v>38.8387781333058</v>
+        <v>-0.490334372010293</v>
       </c>
     </row>
     <row r="65" spans="2:6">
@@ -1917,13 +1929,13 @@
         <v>67</v>
       </c>
       <c r="C65">
-        <v>-0.0134378029651597</v>
+        <v>-1.22484272926519</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>-0.973999595242953</v>
       </c>
       <c r="F65">
-        <v>-0.0710964880268777</v>
+        <v>-0.490334372010293</v>
       </c>
     </row>
     <row r="66" spans="2:6">
@@ -1931,10 +1943,10 @@
         <v>68</v>
       </c>
       <c r="C66">
-        <v>0.280508023505043</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>0.584990421545994</v>
+        <v>0</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -1945,13 +1957,13 @@
         <v>69</v>
       </c>
       <c r="C67">
-        <v>0.701404907815189</v>
+        <v>0</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
       <c r="F67">
-        <v>1.35840763547731</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="2:6">
@@ -1959,7 +1971,7 @@
         <v>70</v>
       </c>
       <c r="C68">
-        <v>0.016193635550666</v>
+        <v>0</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -1973,13 +1985,13 @@
         <v>71</v>
       </c>
       <c r="C69">
-        <v>0.0134378029651597</v>
+        <v>0.037860644946982</v>
       </c>
       <c r="D69">
         <v>0</v>
       </c>
       <c r="F69">
-        <v>0.0710964880268777</v>
+        <v>0.1251208136927</v>
       </c>
     </row>
     <row r="70" spans="2:6">
@@ -1987,13 +1999,13 @@
         <v>72</v>
       </c>
       <c r="C70">
-        <v>0.280508023505043</v>
+        <v>-0.685115350202667</v>
       </c>
       <c r="D70">
-        <v>0.584990421545994</v>
+        <v>-0.509908922243992</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>-0.328860960565215</v>
       </c>
     </row>
     <row r="71" spans="2:6">
@@ -2001,13 +2013,13 @@
         <v>73</v>
       </c>
       <c r="C71">
-        <v>0.701404907815189</v>
+        <v>0.179142093274584</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>0.149726942198534</v>
       </c>
       <c r="F71">
-        <v>1.35840763547731</v>
+        <v>0.0215518982970114</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2015,13 +2027,13 @@
         <v>74</v>
       </c>
       <c r="C72">
-        <v>0.016193635550666</v>
+        <v>-11.4713681888546</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>-0.977944198774425</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>-7.66791228450121</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2029,13 +2041,13 @@
         <v>75</v>
       </c>
       <c r="C73">
-        <v>0.0134378029651597</v>
+        <v>0.037860644946982</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="F73">
-        <v>0.0710964880268777</v>
+        <v>0.1251208136927</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2043,10 +2055,10 @@
         <v>76</v>
       </c>
       <c r="C74">
-        <v>0.0438318116106969</v>
+        <v>0.685115350202667</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>13.9745047656115</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -2057,13 +2069,13 @@
         <v>77</v>
       </c>
       <c r="C75">
-        <v>0.701404907815189</v>
+        <v>-0.217002738221565</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>-0.149726942198532</v>
       </c>
       <c r="F75">
-        <v>1.35840763547731</v>
+        <v>-0.146672711989715</v>
       </c>
     </row>
     <row r="76" spans="2:6">
@@ -2071,13 +2083,13 @@
         <v>78</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>21.7102639547712</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>0.977944198774425</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>1.70788681778017</v>
       </c>
     </row>
     <row r="77" spans="2:6">
@@ -2085,13 +2097,13 @@
         <v>79</v>
       </c>
       <c r="C77">
-        <v>0.0134378029651597</v>
+        <v>0</v>
       </c>
       <c r="D77">
         <v>0</v>
       </c>
       <c r="F77">
-        <v>0.0710964880268777</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="2:6">
@@ -2102,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>0.47366383984469</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -2113,13 +2125,13 @@
         <v>81</v>
       </c>
       <c r="C79">
-        <v>0.700751133690586</v>
+        <v>0.732272158230354</v>
       </c>
       <c r="D79">
-        <v>1.4017205322421</v>
+        <v>0.613817615197493</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>0.552894781801512</v>
       </c>
     </row>
     <row r="80" spans="2:6">
@@ -2133,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>-0.00529407316065884</v>
       </c>
     </row>
     <row r="81" spans="2:6">
@@ -2141,13 +2153,13 @@
         <v>83</v>
       </c>
       <c r="C81">
-        <v>0.000934248204846116</v>
+        <v>0.0236794188830509</v>
       </c>
       <c r="D81">
         <v>0</v>
       </c>
       <c r="F81">
-        <v>0.00184200605052535</v>
+        <v>0.0625604068463566</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2158,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>-0.47366383984469</v>
       </c>
       <c r="F82">
         <v>0</v>
@@ -2169,13 +2181,13 @@
         <v>85</v>
       </c>
       <c r="C83">
-        <v>0.700751133690586</v>
+        <v>-0.732272158230354</v>
       </c>
       <c r="D83">
-        <v>1.4017205322421</v>
+        <v>-0.613817615197493</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>-0.552894781801512</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2183,13 +2195,13 @@
         <v>86</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>55.6811133816782</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>18.5829163097497</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>25.6142170618823</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2197,13 +2209,13 @@
         <v>87</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>-0.0236794188830509</v>
       </c>
       <c r="D85">
         <v>0</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>-0.0625604068463566</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2211,13 +2223,13 @@
         <v>88</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>0.202186882326852</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
       <c r="F86">
-        <v>0.215207705739295</v>
+        <v>1.22740870989835</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2225,13 +2237,13 @@
         <v>89</v>
       </c>
       <c r="C87">
-        <v>0.591599801757736</v>
+        <v>0.732272158230347</v>
       </c>
       <c r="D87">
-        <v>0.833333333333333</v>
+        <v>0.613817615197425</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>0.552894781801512</v>
       </c>
     </row>
     <row r="88" spans="2:6">
@@ -2239,10 +2251,10 @@
         <v>90</v>
       </c>
       <c r="C88">
-        <v>0.109151331932851</v>
+        <v>0.0364356799880509</v>
       </c>
       <c r="D88">
-        <v>1.16375775537515e-09</v>
+        <v>-0.855577918489514</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -2253,13 +2265,13 @@
         <v>91</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>0.0171396787125336</v>
       </c>
       <c r="D89">
-        <v>0.568387197745019</v>
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>-0.215207705739295</v>
+        <v>0.0625604068463566</v>
       </c>
     </row>
     <row r="90" spans="2:6">
@@ -2267,13 +2279,13 @@
         <v>92</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>0.202186882326852</v>
       </c>
       <c r="D90">
         <v>0</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>1.22740870989835</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -2281,13 +2293,13 @@
         <v>93</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>0.732272158230347</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>0.613817615197425</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>0.552894781801512</v>
       </c>
     </row>
     <row r="92" spans="2:6">
@@ -2295,10 +2307,10 @@
         <v>94</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>0.0364356799880509</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>-0.855577918489514</v>
       </c>
       <c r="F92">
         <v>0</v>
@@ -2309,13 +2321,13 @@
         <v>95</v>
       </c>
       <c r="C93">
-        <v>0.556876910144288</v>
+        <v>0.0171396787125336</v>
       </c>
       <c r="D93">
-        <v>0.668091383032151</v>
+        <v>0</v>
       </c>
       <c r="F93">
-        <v>0.449960217429047</v>
+        <v>0.0625604068463566</v>
       </c>
     </row>
     <row r="94" spans="2:6">
@@ -2337,13 +2349,13 @@
         <v>97</v>
       </c>
       <c r="C95">
-        <v>0.556876910144288</v>
+        <v>0.675127312438851</v>
       </c>
       <c r="D95">
-        <v>0.668091383032151</v>
+        <v>0.613817615197425</v>
       </c>
       <c r="F95">
-        <v>0.449960217429047</v>
+        <v>0.552894781801537</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -2351,7 +2363,7 @@
         <v>98</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>0.0211762926426279</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -2365,13 +2377,13 @@
         <v>99</v>
       </c>
       <c r="C97">
-        <v>0.556876910144288</v>
+        <v>0.0162054305077117</v>
       </c>
       <c r="D97">
-        <v>0.668091383032151</v>
+        <v>0</v>
       </c>
       <c r="F97">
-        <v>0.449960217429047</v>
+        <v>0.0625604068463552</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -2379,13 +2391,13 @@
         <v>100</v>
       </c>
       <c r="C98">
-        <v>0.0062283213656528</v>
+        <v>0</v>
       </c>
       <c r="D98">
         <v>0</v>
       </c>
       <c r="F98">
-        <v>0.0122800403368357</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -2393,13 +2405,13 @@
         <v>101</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>0.677241165857167</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>0.613817615197438</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>0.67649274391933</v>
       </c>
     </row>
     <row r="100" spans="2:6">
@@ -2407,13 +2419,13 @@
         <v>102</v>
       </c>
       <c r="C100">
-        <v>2.08452318967125</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>3.28857904406281</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>1.83442441974848</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="2:6">
@@ -2421,13 +2433,13 @@
         <v>103</v>
       </c>
       <c r="C101">
-        <v>1.35253209064382</v>
+        <v>0.000934248204821818</v>
       </c>
       <c r="D101">
-        <v>0.823740894301542</v>
+        <v>0</v>
       </c>
       <c r="F101">
-        <v>1.88314835303429</v>
+        <v>0.000934248204821818</v>
       </c>
     </row>
     <row r="102" spans="2:6">
@@ -2435,13 +2447,13 @@
         <v>104</v>
       </c>
       <c r="C102">
-        <v>-0.00529407316079467</v>
+        <v>0</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
       <c r="F102">
-        <v>-0.0104380342863105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="2:6">
@@ -2449,13 +2461,13 @@
         <v>105</v>
       </c>
       <c r="C103">
-        <v>-0.0153062993748519</v>
+        <v>0.677241165857167</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>0.613817615197438</v>
       </c>
       <c r="F103">
-        <v>-0.0747805001279282</v>
+        <v>0.67649274391933</v>
       </c>
     </row>
     <row r="104" spans="2:6">
@@ -2463,13 +2475,13 @@
         <v>106</v>
       </c>
       <c r="C104">
-        <v>0.470861095242467</v>
+        <v>0</v>
       </c>
       <c r="D104">
         <v>0</v>
       </c>
       <c r="F104">
-        <v>0.552056282648184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="2:6">
@@ -2477,13 +2489,13 @@
         <v>107</v>
       </c>
       <c r="C105">
-        <v>-0.701404907815189</v>
+        <v>-2.73677108753034e-09</v>
       </c>
       <c r="D105">
         <v>0</v>
       </c>
       <c r="F105">
-        <v>-1.35840763547731</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="2:6">
@@ -2491,13 +2503,13 @@
         <v>108</v>
       </c>
       <c r="C106">
-        <v>2.43902274639269</v>
+        <v>0.109151331930016</v>
       </c>
       <c r="D106">
-        <v>3.25215629977101</v>
+        <v>0</v>
       </c>
       <c r="F106">
-        <v>1.57386397408644</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="2:6">
@@ -2505,46 +2517,46 @@
         <v>109</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.568089831190381</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>0.613817615197437</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>0.567341411989326</v>
       </c>
     </row>
     <row r="108" spans="2:6">
       <c r="B108" s="1" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="C108">
-        <v>-1.20180361751539</v>
+        <v>0</v>
       </c>
       <c r="D108">
-        <v>-1.09649645075465</v>
+        <v>0</v>
       </c>
       <c r="F108">
-        <v>-1.28731114745042</v>
+        <v>0.109151331930005</v>
       </c>
     </row>
     <row r="109" spans="2:6">
       <c r="B109" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C109">
-        <v>-0.610192041688615</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>-0.366093156307216</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>-0.764718265243202</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:6">
       <c r="B110" s="1" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2558,21 +2570,21 @@
     </row>
     <row r="111" spans="2:6">
       <c r="B111" s="1" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="C111">
-        <v>0.171278837555121</v>
+        <v>0</v>
       </c>
       <c r="D111">
-        <v>-0.091523289076804</v>
+        <v>0</v>
       </c>
       <c r="F111">
-        <v>0.345831275374102</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:6">
       <c r="B112" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2586,164 +2598,164 @@
     </row>
     <row r="113" spans="2:6">
       <c r="B113" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C113">
-        <v>0.318533823809467</v>
+        <v>0.533366939577836</v>
       </c>
       <c r="D113">
-        <v>0.183046578153608</v>
+        <v>0.613817615197437</v>
       </c>
       <c r="F113">
-        <v>0.453455620648478</v>
+        <v>0.532618520376782</v>
       </c>
     </row>
     <row r="114" spans="2:6">
       <c r="B114" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C114">
-        <v>6.58367936517131</v>
+        <v>0</v>
       </c>
       <c r="D114">
-        <v>6.20572159227754</v>
+        <v>0</v>
       </c>
       <c r="F114">
-        <v>6.8206456536482</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="2:6">
       <c r="B115" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C115">
-        <v>-0.318533823809467</v>
+        <v>0.533366939577836</v>
       </c>
       <c r="D115">
-        <v>-0.183046578153608</v>
+        <v>0.613817615197437</v>
       </c>
       <c r="F115">
-        <v>-0.453455620648478</v>
+        <v>0.532618520376782</v>
       </c>
     </row>
     <row r="116" spans="2:6">
       <c r="B116" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C116">
-        <v>-6.59177618294664</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>-6.21493162253017</v>
+        <v>0</v>
       </c>
       <c r="F116">
-        <v>-6.82739967583346</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="2:6">
       <c r="B117" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C117">
-        <v>0.318533823809467</v>
+        <v>0.533366939577836</v>
       </c>
       <c r="D117">
-        <v>0.183046578153608</v>
+        <v>0.613817615197437</v>
       </c>
       <c r="F117">
-        <v>0.453455620648478</v>
+        <v>0.532618520376781</v>
       </c>
     </row>
     <row r="118" spans="2:6">
       <c r="B118" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C118">
-        <v>-13.175455548118</v>
+        <v>0.00591690529720485</v>
       </c>
       <c r="D118">
-        <v>-12.4206532148077</v>
+        <v>0.00498265709238303</v>
       </c>
       <c r="F118">
-        <v>-13.6480453294817</v>
+        <v>0.00124566427309892</v>
       </c>
     </row>
     <row r="119" spans="2:6">
       <c r="B119" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C119">
-        <v>0.0995342151644687</v>
+        <v>0.000311416068273939</v>
       </c>
       <c r="D119">
-        <v>0.233620088513059</v>
+        <v>0</v>
       </c>
       <c r="F119">
-        <v>-0.0340259449060238</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="2:6">
       <c r="B120" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>0.505699742881324</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>5.29307657444287</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>18.9180536010938</v>
       </c>
     </row>
     <row r="121" spans="2:6">
       <c r="B121" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C121">
-        <v>0.537533432454465</v>
+        <v>1.40064976657272</v>
       </c>
       <c r="D121">
-        <v>0.132473067794157</v>
+        <v>1.22763523039493</v>
       </c>
       <c r="F121">
-        <v>0.940937186202981</v>
+        <v>1.30121256354323</v>
       </c>
     </row>
     <row r="122" spans="2:6">
       <c r="B122" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C122">
-        <v>6.57963095628364</v>
+        <v>0</v>
       </c>
       <c r="D122">
-        <v>6.20019557412597</v>
+        <v>0</v>
       </c>
       <c r="F122">
-        <v>6.81818964558084</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="2:6">
       <c r="B123" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C123">
-        <v>-0.318533823809467</v>
+        <v>-0.0327104875997666</v>
       </c>
       <c r="D123">
-        <v>-0.183046578153608</v>
+        <v>0</v>
       </c>
       <c r="F123">
-        <v>-0.453455620648478</v>
+        <v>-0.0644289032559983</v>
       </c>
     </row>
     <row r="124" spans="2:6">
       <c r="B124" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>1.35815460603964</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -2754,27 +2766,27 @@
     </row>
     <row r="125" spans="2:6">
       <c r="B125" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>-0.732272158230353</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>-0.613817615197493</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>-0.552894781801512</v>
       </c>
     </row>
     <row r="126" spans="2:6">
       <c r="B126" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>6.12017588947213</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>2.12241204138132</v>
       </c>
       <c r="F126">
         <v>0</v>
@@ -2782,49 +2794,49 @@
     </row>
     <row r="127" spans="2:6">
       <c r="B127" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C127">
-        <v>0.418068038973936</v>
+        <v>0</v>
       </c>
       <c r="D127">
-        <v>0.416666666666667</v>
+        <v>0</v>
       </c>
       <c r="F127">
-        <v>0.419429675742455</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="2:6">
       <c r="B128" s="1" t="s">
-        <v>127</v>
+        <v>66</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>-1.22484272926519</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>-0.973999595242953</v>
       </c>
       <c r="F128">
-        <v>0</v>
+        <v>-0.490334372010293</v>
       </c>
     </row>
     <row r="129" spans="2:6">
       <c r="B129" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C129">
-        <v>0.537533432454465</v>
+        <v>-0.606498680495976</v>
       </c>
       <c r="D129">
-        <v>0.132473067794157</v>
+        <v>-0.628727461600854</v>
       </c>
       <c r="F129">
-        <v>0.940937186202981</v>
+        <v>-0.519098715644188</v>
       </c>
     </row>
     <row r="130" spans="2:6">
       <c r="B130" s="1" t="s">
-        <v>129</v>
+        <v>64</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -2833,21 +2845,21 @@
         <v>0</v>
       </c>
       <c r="F130">
-        <v>0</v>
+        <v>-0.153654532606541</v>
       </c>
     </row>
     <row r="131" spans="2:6">
       <c r="B131" s="1" t="s">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="C131">
-        <v>0.418068038973936</v>
+        <v>0.179142093274584</v>
       </c>
       <c r="D131">
-        <v>0.416666666666667</v>
+        <v>0.149726942198534</v>
       </c>
       <c r="F131">
-        <v>0.419429675742455</v>
+        <v>0.0215518982970114</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -2858,7 +2870,7 @@
         <v>0</v>
       </c>
       <c r="D132">
-        <v>0</v>
+        <v>0.00114185891700314</v>
       </c>
       <c r="F132">
         <v>0</v>
@@ -2869,13 +2881,13 @@
         <v>132</v>
       </c>
       <c r="C133">
-        <v>0.537533432454465</v>
+        <v>0.322413224772684</v>
       </c>
       <c r="D133">
-        <v>0.132473067794157</v>
+        <v>0.314363730800427</v>
       </c>
       <c r="F133">
-        <v>0.940937186202981</v>
+        <v>0.322109764668444</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -2883,13 +2895,13 @@
         <v>133</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>10.2388957659167</v>
       </c>
       <c r="D134">
-        <v>0</v>
+        <v>-0.00114185891700314</v>
       </c>
       <c r="F134">
-        <v>0</v>
+        <v>7.17570941608127</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -2897,13 +2909,13 @@
         <v>134</v>
       </c>
       <c r="C135">
-        <v>0.537533432454465</v>
+        <v>-0.322413224772684</v>
       </c>
       <c r="D135">
-        <v>0.132473067794157</v>
+        <v>-0.314363730800427</v>
       </c>
       <c r="F135">
-        <v>0.940937186202981</v>
+        <v>-0.322109764668444</v>
       </c>
     </row>
     <row r="136" spans="2:6">
@@ -2911,13 +2923,13 @@
         <v>135</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>-10.2465254595894</v>
       </c>
       <c r="D136">
-        <v>0</v>
+        <v>-0.00508646244847566</v>
       </c>
       <c r="F136">
-        <v>0</v>
+        <v>-7.17757791249091</v>
       </c>
     </row>
     <row r="137" spans="2:6">
@@ -2925,13 +2937,13 @@
         <v>136</v>
       </c>
       <c r="C137">
-        <v>0.418068038973936</v>
+        <v>0.321946100670274</v>
       </c>
       <c r="D137">
-        <v>0.416666666666667</v>
+        <v>0.314363730800427</v>
       </c>
       <c r="F137">
-        <v>0.419429675742455</v>
+        <v>0.322109764668444</v>
       </c>
     </row>
     <row r="138" spans="2:6">
@@ -2939,13 +2951,13 @@
         <v>137</v>
       </c>
       <c r="C138">
-        <v>4.54993844785086</v>
+        <v>-20.4854212255061</v>
       </c>
       <c r="D138">
-        <v>4.28857904406281</v>
+        <v>-0.00394460353146859</v>
       </c>
       <c r="F138">
-        <v>5.71248136453328</v>
+        <v>-14.3532873285722</v>
       </c>
     </row>
     <row r="139" spans="2:6">
@@ -2953,13 +2965,13 @@
         <v>138</v>
       </c>
       <c r="C139">
-        <v>4.54993844785086</v>
+        <v>0.095343398132941</v>
       </c>
       <c r="D139">
-        <v>4.28857904406281</v>
+        <v>0.10230293586624</v>
       </c>
       <c r="F139">
-        <v>5.71248136453328</v>
+        <v>0.0945569019982185</v>
       </c>
     </row>
     <row r="140" spans="2:6">
@@ -2981,13 +2993,13 @@
         <v>140</v>
       </c>
       <c r="C141">
-        <v>0.556876910144288</v>
+        <v>0.549015927310017</v>
       </c>
       <c r="D141">
-        <v>0.668091383032151</v>
+        <v>0.526424525734615</v>
       </c>
       <c r="F141">
-        <v>0.449960217429047</v>
+        <v>0.549662627338669</v>
       </c>
     </row>
     <row r="142" spans="2:6">
@@ -2995,13 +3007,13 @@
         <v>141</v>
       </c>
       <c r="C142">
-        <v>2.27496922392543</v>
+        <v>10.2351587730974</v>
       </c>
       <c r="D142">
-        <v>2.1442895220314</v>
+        <v>-0.00394460353146859</v>
       </c>
       <c r="F142">
-        <v>2.85624068226664</v>
+        <v>7.17446375180817</v>
       </c>
     </row>
     <row r="143" spans="2:6">
@@ -3009,13 +3021,13 @@
         <v>142</v>
       </c>
       <c r="C143">
-        <v>1.5964422891452</v>
+        <v>-0.322724640840958</v>
       </c>
       <c r="D143">
-        <v>1.78082209630397</v>
+        <v>-0.314363730800427</v>
       </c>
       <c r="F143">
-        <v>1.41701547764513</v>
+        <v>-0.322109764668448</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -3023,13 +3035,13 @@
         <v>143</v>
       </c>
       <c r="C144">
-        <v>4.54993844785086</v>
+        <v>0</v>
       </c>
       <c r="D144">
-        <v>4.28857904406281</v>
+        <v>0</v>
       </c>
       <c r="F144">
-        <v>5.71248136453328</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -3037,13 +3049,13 @@
         <v>144</v>
       </c>
       <c r="C145">
-        <v>3.19288457829039</v>
+        <v>0</v>
       </c>
       <c r="D145">
-        <v>3.56164419260795</v>
+        <v>0</v>
       </c>
       <c r="F145">
-        <v>2.83403095529025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -3062,21 +3074,21 @@
     </row>
     <row r="147" spans="2:6">
       <c r="B147" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C147">
-        <v>0</v>
+        <v>0.418068038973899</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="F147">
-        <v>0</v>
+        <v>0.416666666666667</v>
       </c>
     </row>
     <row r="148" spans="2:6">
       <c r="B148" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -3090,282 +3102,282 @@
     </row>
     <row r="149" spans="2:6">
       <c r="B149" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>0.549015927310017</v>
       </c>
       <c r="D149">
-        <v>0</v>
+        <v>0.526424525734615</v>
       </c>
       <c r="F149">
-        <v>0</v>
+        <v>0.549662627338669</v>
       </c>
     </row>
     <row r="150" spans="2:6">
       <c r="B150" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C150">
-        <v>24.25</v>
+        <v>0</v>
       </c>
       <c r="D150">
-        <v>24.25</v>
+        <v>0</v>
       </c>
       <c r="F150">
-        <v>24.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="2:6">
       <c r="B151" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>0.418068038973899</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="F151">
-        <v>0</v>
+        <v>0.416666666666667</v>
       </c>
     </row>
     <row r="152" spans="2:6">
       <c r="B152" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C152">
-        <v>48.5</v>
+        <v>0</v>
       </c>
       <c r="D152">
-        <v>48.5</v>
+        <v>0</v>
       </c>
       <c r="F152">
-        <v>48.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="2:6">
       <c r="B153" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>0.549015927310017</v>
       </c>
       <c r="D153">
-        <v>0</v>
+        <v>0.526424525734615</v>
       </c>
       <c r="F153">
-        <v>0</v>
+        <v>0.549662627338669</v>
       </c>
     </row>
     <row r="154" spans="2:6">
       <c r="B154" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C154">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="D154">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="F154">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="2:6">
       <c r="B155" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>0.549015927310017</v>
       </c>
       <c r="D155">
-        <v>0</v>
+        <v>0.526424525734615</v>
       </c>
       <c r="F155">
-        <v>0</v>
+        <v>0.549662627338669</v>
       </c>
     </row>
     <row r="156" spans="2:6">
       <c r="B156" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C156">
-        <v>44.2542190794519</v>
+        <v>0</v>
       </c>
       <c r="D156">
-        <v>46.0002669508854</v>
+        <v>0</v>
       </c>
       <c r="F156">
-        <v>42.6114265740454</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="2:6">
       <c r="B157" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>0.418068038973899</v>
       </c>
       <c r="D157">
-        <v>0</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="F157">
-        <v>0</v>
+        <v>0.416666666666667</v>
       </c>
     </row>
     <row r="158" spans="2:6">
       <c r="B158" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>6.65195672807139</v>
       </c>
       <c r="D158">
-        <v>0</v>
+        <v>5.29307657444287</v>
       </c>
       <c r="F158">
-        <v>0</v>
+        <v>21.0696608988758</v>
       </c>
     </row>
     <row r="159" spans="2:6">
       <c r="B159" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>6.65195672807139</v>
       </c>
       <c r="D159">
-        <v>0</v>
+        <v>5.29307657444287</v>
       </c>
       <c r="F159">
-        <v>0</v>
+        <v>21.0696608988758</v>
       </c>
     </row>
     <row r="160" spans="2:6">
       <c r="B160" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C160">
-        <v>-0.513836512665364</v>
+        <v>0</v>
       </c>
       <c r="D160">
         <v>0</v>
       </c>
       <c r="F160">
-        <v>-1.01310332778894</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="2:6">
       <c r="B161" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C161">
-        <v>-0.171278837555121</v>
+        <v>0.533366939577836</v>
       </c>
       <c r="D161">
-        <v>0</v>
+        <v>0.613817615197437</v>
       </c>
       <c r="F161">
-        <v>-0.33770110926298</v>
+        <v>0.532618520376781</v>
       </c>
     </row>
     <row r="162" spans="2:6">
       <c r="B162" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C162">
-        <v>-0.0226555189675183</v>
+        <v>3.3259783640357</v>
       </c>
       <c r="D162">
-        <v>0</v>
+        <v>2.64653828722143</v>
       </c>
       <c r="F162">
-        <v>-0.0446686467252396</v>
+        <v>10.5348304494379</v>
       </c>
     </row>
     <row r="163" spans="2:6">
       <c r="B163" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C163">
-        <v>-0.00755183965583944</v>
+        <v>1.64043467209609</v>
       </c>
       <c r="D163">
-        <v>0</v>
+        <v>1.53454403799362</v>
       </c>
       <c r="F163">
-        <v>-0.0148895489084132</v>
+        <v>1.53439494241387</v>
       </c>
     </row>
     <row r="164" spans="2:6">
       <c r="B164" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C164">
-        <v>-0.00373699281938446</v>
+        <v>6.65195672807139</v>
       </c>
       <c r="D164">
-        <v>0</v>
+        <v>5.29307657444287</v>
       </c>
       <c r="F164">
-        <v>-0.00736802420210138</v>
+        <v>21.0696608988758</v>
       </c>
     </row>
     <row r="165" spans="2:6">
       <c r="B165" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C165">
-        <v>-0.00124566427312816</v>
+        <v>3.28086934419218</v>
       </c>
       <c r="D165">
-        <v>0</v>
+        <v>3.06908807598724</v>
       </c>
       <c r="F165">
-        <v>-0.00245600806736713</v>
+        <v>3.06878988482774</v>
       </c>
     </row>
     <row r="166" spans="2:6">
       <c r="B166" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C166">
-        <v>-0.0221883948650953</v>
+        <v>0</v>
       </c>
       <c r="D166">
         <v>0</v>
       </c>
       <c r="F166">
-        <v>-0.043747643699977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="2:6">
       <c r="B167" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C167">
-        <v>-0.00739613162169842</v>
+        <v>0</v>
       </c>
       <c r="D167">
         <v>0</v>
       </c>
       <c r="F167">
-        <v>-0.0145825478999923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="2:6">
       <c r="B168" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C168">
-        <v>-0.0266260738381143</v>
+        <v>0</v>
       </c>
       <c r="D168">
         <v>0</v>
       </c>
       <c r="F168">
-        <v>-0.0524971724399724</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="2:6">
@@ -3373,13 +3385,13 @@
         <v>166</v>
       </c>
       <c r="C169">
-        <v>-0.0088753579460381</v>
+        <v>0</v>
       </c>
       <c r="D169">
         <v>0</v>
       </c>
       <c r="F169">
-        <v>-0.0174990574799908</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="2:6">
@@ -3387,13 +3399,13 @@
         <v>167</v>
       </c>
       <c r="C170">
-        <v>-0.0775426010022277</v>
+        <v>36.3691920828002</v>
       </c>
       <c r="D170">
-        <v>0</v>
+        <v>23.2068820931237</v>
       </c>
       <c r="F170">
-        <v>-0.152886502193604</v>
+        <v>14.9721819955637</v>
       </c>
     </row>
     <row r="171" spans="2:6">
@@ -3401,13 +3413,13 @@
         <v>168</v>
       </c>
       <c r="C171">
-        <v>-0.0258475336674092</v>
+        <v>0</v>
       </c>
       <c r="D171">
         <v>0</v>
       </c>
       <c r="F171">
-        <v>-0.0509621673978679</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="2:6">
@@ -3415,13 +3427,13 @@
         <v>169</v>
       </c>
       <c r="C172">
-        <v>-0.0016349343584807</v>
+        <v>72.7383841656004</v>
       </c>
       <c r="D172">
-        <v>0</v>
+        <v>46.4137641862475</v>
       </c>
       <c r="F172">
-        <v>-0.00322351058841935</v>
+        <v>62.8831643813676</v>
       </c>
     </row>
     <row r="173" spans="2:6">
@@ -3429,13 +3441,13 @@
         <v>170</v>
       </c>
       <c r="C173">
-        <v>-0.000544978119493568</v>
+        <v>0</v>
       </c>
       <c r="D173">
         <v>0</v>
       </c>
       <c r="F173">
-        <v>-0.00107450352947312</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="2:6">
@@ -3443,13 +3455,13 @@
         <v>171</v>
       </c>
       <c r="C174">
-        <v>-0.0179842779432877</v>
+        <v>145.476768331201</v>
       </c>
       <c r="D174">
-        <v>0</v>
+        <v>92.827528372495</v>
       </c>
       <c r="F174">
-        <v>-0.0354586164726129</v>
+        <v>125.766328762735</v>
       </c>
     </row>
     <row r="175" spans="2:6">
@@ -3457,13 +3469,13 @@
         <v>172</v>
       </c>
       <c r="C175">
-        <v>-0.00599475931442925</v>
+        <v>0</v>
       </c>
       <c r="D175">
         <v>0</v>
       </c>
       <c r="F175">
-        <v>-0.0118195388242043</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="2:6">
@@ -3471,13 +3483,13 @@
         <v>173</v>
       </c>
       <c r="C176">
-        <v>-0.00140137230726917</v>
+        <v>64.803586846296</v>
       </c>
       <c r="D176">
-        <v>0</v>
+        <v>44.5018890618584</v>
       </c>
       <c r="F176">
-        <v>-0.00276300907578802</v>
+        <v>27.9270688970819</v>
       </c>
     </row>
     <row r="177" spans="2:6">
@@ -3485,13 +3497,13 @@
         <v>174</v>
       </c>
       <c r="C177">
-        <v>-0.000467124102423058</v>
+        <v>0</v>
       </c>
       <c r="D177">
         <v>0</v>
       </c>
       <c r="F177">
-        <v>-0.000921003025262673</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="2:6">
@@ -3499,13 +3511,13 @@
         <v>175</v>
       </c>
       <c r="C178">
-        <v>-0.000934248204846116</v>
+        <v>0</v>
       </c>
       <c r="D178">
         <v>0</v>
       </c>
       <c r="F178">
-        <v>-0.00184200605052535</v>
+        <v>32.9388003902402</v>
       </c>
     </row>
     <row r="179" spans="2:6">
@@ -3513,13 +3525,13 @@
         <v>176</v>
       </c>
       <c r="C179">
-        <v>-0.000311416068282039</v>
+        <v>0</v>
       </c>
       <c r="D179">
         <v>0</v>
       </c>
       <c r="F179">
-        <v>-0.000614002016841782</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="2:6">
@@ -3527,13 +3539,13 @@
         <v>177</v>
       </c>
       <c r="C180">
-        <v>-0.00280274461453835</v>
+        <v>-0.513836512652</v>
       </c>
       <c r="D180">
         <v>0</v>
       </c>
       <c r="F180">
-        <v>-0.00552601815157604</v>
+        <v>-0.513836512652</v>
       </c>
     </row>
     <row r="181" spans="2:6">
@@ -3541,13 +3553,13 @@
         <v>178</v>
       </c>
       <c r="C181">
-        <v>-0.000934248204846116</v>
+        <v>-0.171278837550667</v>
       </c>
       <c r="D181">
         <v>0</v>
       </c>
       <c r="F181">
-        <v>-0.00184200605052535</v>
+        <v>-0.171278837550667</v>
       </c>
     </row>
     <row r="182" spans="2:6">
@@ -3555,13 +3567,13 @@
         <v>179</v>
       </c>
       <c r="C182">
-        <v>-0.00280274461453835</v>
+        <v>-0.0226555189669291</v>
       </c>
       <c r="D182">
         <v>0</v>
       </c>
       <c r="F182">
-        <v>-0.00552601815157604</v>
+        <v>-0.0226555189669291</v>
       </c>
     </row>
     <row r="183" spans="2:6">
@@ -3569,13 +3581,13 @@
         <v>180</v>
       </c>
       <c r="C183">
-        <v>-0.000934248204846116</v>
+        <v>-0.00755183965564303</v>
       </c>
       <c r="D183">
         <v>0</v>
       </c>
       <c r="F183">
-        <v>-0.00184200605052535</v>
+        <v>-0.00755183965564303</v>
       </c>
     </row>
     <row r="184" spans="2:6">
@@ -3583,13 +3595,13 @@
         <v>181</v>
       </c>
       <c r="C184">
-        <v>-0.00420411692180752</v>
+        <v>-0.00373699281928727</v>
       </c>
       <c r="D184">
         <v>0</v>
       </c>
       <c r="F184">
-        <v>-0.00828902722736406</v>
+        <v>-0.00373699281928727</v>
       </c>
     </row>
     <row r="185" spans="2:6">
@@ -3597,13 +3609,13 @@
         <v>182</v>
       </c>
       <c r="C185">
-        <v>-0.00140137230726917</v>
+        <v>-0.00124566427309576</v>
       </c>
       <c r="D185">
         <v>0</v>
       </c>
       <c r="F185">
-        <v>-0.00276300907578802</v>
+        <v>-0.00124566427309576</v>
       </c>
     </row>
     <row r="186" spans="2:6">
@@ -3611,13 +3623,13 @@
         <v>183</v>
       </c>
       <c r="C186">
-        <v>-0.0016349343584807</v>
+        <v>-0.0221883948645182</v>
       </c>
       <c r="D186">
         <v>0</v>
       </c>
       <c r="F186">
-        <v>-0.00322351058841935</v>
+        <v>-0.0221883948645182</v>
       </c>
     </row>
     <row r="187" spans="2:6">
@@ -3625,13 +3637,13 @@
         <v>184</v>
       </c>
       <c r="C187">
-        <v>-0.000544978119493568</v>
+        <v>-0.00739613162150606</v>
       </c>
       <c r="D187">
         <v>0</v>
       </c>
       <c r="F187">
-        <v>-0.00107450352947312</v>
+        <v>-0.00739613162150606</v>
       </c>
     </row>
     <row r="188" spans="2:6">
@@ -3639,13 +3651,13 @@
         <v>185</v>
       </c>
       <c r="C188">
-        <v>-0.00256918256332682</v>
+        <v>-0.0266260738374218</v>
       </c>
       <c r="D188">
         <v>0</v>
       </c>
       <c r="F188">
-        <v>-0.0050655166389447</v>
+        <v>-0.0266260738374218</v>
       </c>
     </row>
     <row r="189" spans="2:6">
@@ -3653,13 +3665,13 @@
         <v>186</v>
       </c>
       <c r="C189">
-        <v>-0.000856394187775606</v>
+        <v>-0.00887535794580727</v>
       </c>
       <c r="D189">
         <v>0</v>
       </c>
       <c r="F189">
-        <v>-0.0016885055463149</v>
+        <v>-0.00887535794580727</v>
       </c>
     </row>
     <row r="190" spans="2:6">
@@ -3667,13 +3679,13 @@
         <v>187</v>
       </c>
       <c r="C190">
-        <v>-0.0130794748678456</v>
+        <v>-0.0775426010002109</v>
       </c>
       <c r="D190">
         <v>0</v>
       </c>
       <c r="F190">
-        <v>-0.0257880847073548</v>
+        <v>-0.0775426010002109</v>
       </c>
     </row>
     <row r="191" spans="2:6">
@@ -3681,13 +3693,13 @@
         <v>188</v>
       </c>
       <c r="C191">
-        <v>-0.00435982495594854</v>
+        <v>-0.025847533666737</v>
       </c>
       <c r="D191">
         <v>0</v>
       </c>
       <c r="F191">
-        <v>-0.00859602823578495</v>
+        <v>-0.025847533666737</v>
       </c>
     </row>
     <row r="192" spans="2:6">
@@ -3695,13 +3707,13 @@
         <v>189</v>
       </c>
       <c r="C192">
-        <v>-0.00210205846090376</v>
+        <v>-0.00163493435843818</v>
       </c>
       <c r="D192">
         <v>0</v>
       </c>
       <c r="F192">
-        <v>-0.00414451361368203</v>
+        <v>-0.00163493435843818</v>
       </c>
     </row>
     <row r="193" spans="2:6">
@@ -3709,13 +3721,13 @@
         <v>190</v>
       </c>
       <c r="C193">
-        <v>-0.000700686153634587</v>
+        <v>-0.000544978119479394</v>
       </c>
       <c r="D193">
         <v>0</v>
       </c>
       <c r="F193">
-        <v>-0.00138150453789401</v>
+        <v>-0.000544978119479394</v>
       </c>
     </row>
     <row r="194" spans="2:6">
@@ -3723,13 +3735,13 @@
         <v>191</v>
       </c>
       <c r="C194">
-        <v>-0.0056054892290767</v>
+        <v>-0.01798427794282</v>
       </c>
       <c r="D194">
         <v>0</v>
       </c>
       <c r="F194">
-        <v>-0.0110520363031521</v>
+        <v>-0.01798427794282</v>
       </c>
     </row>
     <row r="195" spans="2:6">
@@ -3737,13 +3749,13 @@
         <v>192</v>
       </c>
       <c r="C195">
-        <v>-0.00186849640969223</v>
+        <v>-0.00599475931427333</v>
       </c>
       <c r="D195">
         <v>0</v>
       </c>
       <c r="F195">
-        <v>-0.00368401210105069</v>
+        <v>-0.00599475931427333</v>
       </c>
     </row>
     <row r="196" spans="2:6">
@@ -3751,13 +3763,13 @@
         <v>193</v>
       </c>
       <c r="C196">
-        <v>12.4547568788937</v>
+        <v>-0.00140137230723273</v>
       </c>
       <c r="D196">
-        <v>14.4230680930836</v>
+        <v>0</v>
       </c>
       <c r="F196">
-        <v>10.2189574577454</v>
+        <v>-0.00140137230723273</v>
       </c>
     </row>
     <row r="197" spans="2:6">
@@ -3765,13 +3777,13 @@
         <v>194</v>
       </c>
       <c r="C197">
-        <v>-2.81549531735967</v>
+        <v>-0.000467124102410909</v>
       </c>
       <c r="D197">
-        <v>-4.02067218081343</v>
+        <v>0</v>
       </c>
       <c r="F197">
-        <v>-1.61614894271202</v>
+        <v>-0.000467124102410909</v>
       </c>
     </row>
     <row r="198" spans="2:6">
@@ -3779,13 +3791,13 @@
         <v>195</v>
       </c>
       <c r="C198">
-        <v>-13.316873336924</v>
+        <v>-0.000934248204821818</v>
       </c>
       <c r="D198">
-        <v>-13.8728921821185</v>
+        <v>0</v>
       </c>
       <c r="F198">
-        <v>-12.4689212020849</v>
+        <v>-0.000934248204821818</v>
       </c>
     </row>
     <row r="199" spans="2:6">
@@ -3793,184 +3805,280 @@
         <v>196</v>
       </c>
       <c r="C199">
-        <v>2.8464422891452</v>
+        <v>-0.000311416068273939</v>
       </c>
       <c r="D199">
-        <v>3.03082209630397</v>
+        <v>0</v>
       </c>
       <c r="F199">
-        <v>2.66701547764513</v>
+        <v>-0.000311416068273939</v>
       </c>
     </row>
     <row r="200" spans="2:6">
       <c r="B200" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E200">
-        <v>1.01310332778894</v>
+        <v>197</v>
+      </c>
+      <c r="C200">
+        <v>-0.00280274461446545</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="F200">
+        <v>-0.00280274461446545</v>
       </c>
     </row>
     <row r="201" spans="2:6">
       <c r="B201" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E201">
-        <v>-0.00813016611111095</v>
+        <v>198</v>
+      </c>
+      <c r="C201">
+        <v>-0.000934248204821818</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+      <c r="F201">
+        <v>-0.000934248204821818</v>
       </c>
     </row>
     <row r="202" spans="2:6">
       <c r="B202" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E202">
-        <v>2.65521219723342</v>
+        <v>199</v>
+      </c>
+      <c r="C202">
+        <v>-0.00280274461446545</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="F202">
+        <v>-0.00280274461446545</v>
       </c>
     </row>
     <row r="203" spans="2:6">
       <c r="B203" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E203">
-        <v>0</v>
+        <v>200</v>
+      </c>
+      <c r="C203">
+        <v>-0.000934248204821818</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+      <c r="F203">
+        <v>-0.000934248204821818</v>
       </c>
     </row>
     <row r="204" spans="2:6">
       <c r="B204" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E204">
-        <v>0</v>
+        <v>201</v>
+      </c>
+      <c r="C204">
+        <v>-0.00420411692169818</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="F204">
+        <v>-0.00420411692169818</v>
       </c>
     </row>
     <row r="205" spans="2:6">
       <c r="B205" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E205">
-        <v>0</v>
+        <v>202</v>
+      </c>
+      <c r="C205">
+        <v>-0.00140137230723273</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="F205">
+        <v>-0.00140137230723273</v>
       </c>
     </row>
     <row r="206" spans="2:6">
       <c r="B206" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E206">
-        <v>0</v>
+        <v>203</v>
+      </c>
+      <c r="C206">
+        <v>-0.00163493435843818</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="F206">
+        <v>-0.00163493435843818</v>
       </c>
     </row>
     <row r="207" spans="2:6">
       <c r="B207" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E207">
-        <v>0</v>
+        <v>204</v>
+      </c>
+      <c r="C207">
+        <v>-0.000544978119479394</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="F207">
+        <v>-0.000544978119479394</v>
       </c>
     </row>
     <row r="208" spans="2:6">
       <c r="B208" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E208">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="2:5">
+        <v>205</v>
+      </c>
+      <c r="C208">
+        <v>-0.00256918256326</v>
+      </c>
+      <c r="D208">
+        <v>0</v>
+      </c>
+      <c r="F208">
+        <v>-0.00256918256326</v>
+      </c>
+    </row>
+    <row r="209" spans="2:6">
       <c r="B209" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E209">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="2:5">
+        <v>206</v>
+      </c>
+      <c r="C209">
+        <v>-0.000856394187753333</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="F209">
+        <v>-0.000856394187753333</v>
+      </c>
+    </row>
+    <row r="210" spans="2:6">
       <c r="B210" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E210">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="2:5">
+        <v>207</v>
+      </c>
+      <c r="C210">
+        <v>-0.0130794748675055</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="F210">
+        <v>-0.0130794748675055</v>
+      </c>
+    </row>
+    <row r="211" spans="2:6">
       <c r="B211" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E211">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="2:5">
+        <v>208</v>
+      </c>
+      <c r="C211">
+        <v>-0.00435982495583515</v>
+      </c>
+      <c r="D211">
+        <v>0</v>
+      </c>
+      <c r="F211">
+        <v>-0.00435982495583515</v>
+      </c>
+    </row>
+    <row r="212" spans="2:6">
       <c r="B212" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E212">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="2:5">
+        <v>209</v>
+      </c>
+      <c r="C212">
+        <v>-0.00210205846084909</v>
+      </c>
+      <c r="D212">
+        <v>0</v>
+      </c>
+      <c r="F212">
+        <v>-0.00210205846084909</v>
+      </c>
+    </row>
+    <row r="213" spans="2:6">
       <c r="B213" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E213">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="2:5">
+        <v>210</v>
+      </c>
+      <c r="C213">
+        <v>-0.000700686153616364</v>
+      </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="F213">
+        <v>-0.000700686153616364</v>
+      </c>
+    </row>
+    <row r="214" spans="2:6">
       <c r="B214" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E214">
-        <v>-0.178553130473737</v>
-      </c>
-    </row>
-    <row r="215" spans="2:5">
+        <v>211</v>
+      </c>
+      <c r="C214">
+        <v>-0.00560548922893091</v>
+      </c>
+      <c r="D214">
+        <v>0</v>
+      </c>
+      <c r="F214">
+        <v>-0.00560548922893091</v>
+      </c>
+    </row>
+    <row r="215" spans="2:6">
       <c r="B215" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E215">
-        <v>-0.155649510105642</v>
-      </c>
-    </row>
-    <row r="216" spans="2:5">
+        <v>212</v>
+      </c>
+      <c r="C215">
+        <v>-0.00186849640964364</v>
+      </c>
+      <c r="D215">
+        <v>0</v>
+      </c>
+      <c r="F215">
+        <v>-0.00186849640964364</v>
+      </c>
+    </row>
+    <row r="216" spans="2:6">
       <c r="B216" s="1" t="s">
-        <v>209</v>
+        <v>54</v>
       </c>
       <c r="E216">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="217" spans="2:5">
+        <v>0.360181980045458</v>
+      </c>
+    </row>
+    <row r="217" spans="2:6">
       <c r="B217" s="1" t="s">
-        <v>210</v>
+        <v>55</v>
       </c>
       <c r="E217">
-        <v>-0.435377669529055</v>
-      </c>
-    </row>
-    <row r="218" spans="2:5">
+        <v>0.149726942198534</v>
+      </c>
+    </row>
+    <row r="218" spans="2:6">
       <c r="B218" s="1" t="s">
-        <v>211</v>
+        <v>56</v>
       </c>
       <c r="E218">
-        <v>-2.25768231792258</v>
-      </c>
-    </row>
-    <row r="219" spans="2:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="2:6">
       <c r="B219" s="1" t="s">
-        <v>212</v>
+        <v>57</v>
       </c>
       <c r="E219">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="2:5">
+        <v>0.00217991247791405</v>
+      </c>
+    </row>
+    <row r="220" spans="2:6">
       <c r="B220" s="1" t="s">
         <v>213</v>
       </c>
       <c r="E220">
-        <v>0.00368401210105069</v>
-      </c>
-    </row>
-    <row r="221" spans="2:5">
+        <v>0.00217991247791758</v>
+      </c>
+    </row>
+    <row r="221" spans="2:6">
       <c r="B221" s="1" t="s">
         <v>214</v>
       </c>
@@ -3978,7 +4086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="2:5">
+    <row r="222" spans="2:6">
       <c r="B222" s="1" t="s">
         <v>215</v>
       </c>
@@ -3986,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="2:5">
+    <row r="223" spans="2:6">
       <c r="B223" s="1" t="s">
         <v>216</v>
       </c>
@@ -3994,7 +4102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="2:5">
+    <row r="224" spans="2:6">
       <c r="B224" s="1" t="s">
         <v>217</v>
       </c>
@@ -4031,7 +4139,7 @@
         <v>221</v>
       </c>
       <c r="E228">
-        <v>0.00414451361368203</v>
+        <v>0.00373699281928727</v>
       </c>
     </row>
     <row r="229" spans="2:5">
@@ -4039,7 +4147,7 @@
         <v>222</v>
       </c>
       <c r="E229">
-        <v>0.00138150453789401</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230" spans="2:5">
@@ -4047,7 +4155,7 @@
         <v>223</v>
       </c>
       <c r="E230">
-        <v>1.16376613450852e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231" spans="2:5">
@@ -4055,7 +4163,7 @@
         <v>224</v>
       </c>
       <c r="E231">
-        <v>0.733629148046201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="232" spans="2:5">
@@ -4063,7 +4171,7 @@
         <v>225</v>
       </c>
       <c r="E232">
-        <v>0</v>
+        <v>2.52734481433765</v>
       </c>
     </row>
     <row r="233" spans="2:5">
@@ -4079,7 +4187,7 @@
         <v>227</v>
       </c>
       <c r="E234">
-        <v>0</v>
+        <v>-2.12957461095162</v>
       </c>
     </row>
     <row r="235" spans="2:5">
@@ -4087,6 +4195,134 @@
         <v>228</v>
       </c>
       <c r="E235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="2:5">
+      <c r="B236" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="2:5">
+      <c r="B237" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="2:5">
+      <c r="B238" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E238">
+        <v>0.00560548922893091</v>
+      </c>
+    </row>
+    <row r="239" spans="2:5">
+      <c r="B239" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="2:5">
+      <c r="B240" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E240">
+        <v>0.00342557675101333</v>
+      </c>
+    </row>
+    <row r="241" spans="2:5">
+      <c r="B241" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="2:5">
+      <c r="B242" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E242">
+        <v>0.00373699281928727</v>
+      </c>
+    </row>
+    <row r="243" spans="2:5">
+      <c r="B243" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E243">
+        <v>0.00124566427309576</v>
+      </c>
+    </row>
+    <row r="244" spans="2:5">
+      <c r="B244" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E244">
+        <v>0.00280274461446545</v>
+      </c>
+    </row>
+    <row r="245" spans="2:5">
+      <c r="B245" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="2:5">
+      <c r="B246" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E246">
+        <v>0.04773853675636</v>
+      </c>
+    </row>
+    <row r="247" spans="2:5">
+      <c r="B247" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="2:5">
+      <c r="B248" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E248">
+        <v>0.0314530199507899</v>
+      </c>
+    </row>
+    <row r="249" spans="2:5">
+      <c r="B249" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="2:5">
+      <c r="B250" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E250">
+        <v>0.0202420444378061</v>
+      </c>
+    </row>
+    <row r="251" spans="2:5">
+      <c r="B251" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E251">
         <v>0</v>
       </c>
     </row>

</xml_diff>